<commit_message>
Finish login and exit Ref #111
</commit_message>
<xml_diff>
--- a/database/数据库-业务处理.xlsx
+++ b/database/数据库-业务处理.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22228"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\流宇\Desktop\git\database\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B7021F7-3FD1-4450-BDBE-769AB52F51C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12195"/>
+    <workbookView xWindow="2925" yWindow="1785" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="332">
   <si>
     <t>purchase_request表（请购单）</t>
   </si>
@@ -212,18 +218,6 @@
   </si>
   <si>
     <t>存货属性</t>
-  </si>
-  <si>
-    <t>ts_present_num</t>
-  </si>
-  <si>
-    <t>center_stock表（中心存储物）</t>
-  </si>
-  <si>
-    <t>仓库编号</t>
-  </si>
-  <si>
-    <t>cs_present_num</t>
   </si>
   <si>
     <t>purchase_contract表（采购合同）</t>
@@ -1520,18 +1514,16 @@
   <si>
     <t>默认登录当前时间，可手工调整</t>
   </si>
+  <si>
+    <t>total_present_num</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="22">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1554,345 +1546,21 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
+      <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="17">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -1980,251 +1648,9 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2305,61 +1731,17 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="1" builtinId="52"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="2" builtinId="42"/>
-    <cellStyle name="强调文字颜色 4" xfId="3" builtinId="41"/>
-    <cellStyle name="输入" xfId="4" builtinId="20"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="5" builtinId="39"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="6" builtinId="38"/>
-    <cellStyle name="货币" xfId="7" builtinId="4"/>
-    <cellStyle name="强调文字颜色 3" xfId="8" builtinId="37"/>
-    <cellStyle name="百分比" xfId="9" builtinId="5"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="10" builtinId="36"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="11" builtinId="48"/>
-    <cellStyle name="强调文字颜色 2" xfId="12" builtinId="33"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="13" builtinId="32"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="14" builtinId="44"/>
-    <cellStyle name="计算" xfId="15" builtinId="22"/>
-    <cellStyle name="强调文字颜色 1" xfId="16" builtinId="29"/>
-    <cellStyle name="适中" xfId="17" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="18" builtinId="46"/>
-    <cellStyle name="好" xfId="19" builtinId="26"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="20" builtinId="30"/>
-    <cellStyle name="汇总" xfId="21" builtinId="25"/>
-    <cellStyle name="差" xfId="22" builtinId="27"/>
-    <cellStyle name="检查单元格" xfId="23" builtinId="23"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="标题 1" xfId="25" builtinId="16"/>
-    <cellStyle name="解释性文本" xfId="26" builtinId="53"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="27" builtinId="34"/>
-    <cellStyle name="标题 4" xfId="28" builtinId="19"/>
-    <cellStyle name="货币[0]" xfId="29" builtinId="7"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="30" builtinId="43"/>
-    <cellStyle name="千位分隔" xfId="31" builtinId="3"/>
-    <cellStyle name="已访问的超链接" xfId="32" builtinId="9"/>
-    <cellStyle name="标题" xfId="33" builtinId="15"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="34" builtinId="35"/>
-    <cellStyle name="警告文本" xfId="35" builtinId="11"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
-    <cellStyle name="注释" xfId="37" builtinId="10"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="38" builtinId="50"/>
-    <cellStyle name="强调文字颜色 5" xfId="39" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="40" builtinId="51"/>
-    <cellStyle name="超链接" xfId="41" builtinId="8"/>
-    <cellStyle name="千位分隔[0]" xfId="42" builtinId="6"/>
-    <cellStyle name="标题 2" xfId="43" builtinId="17"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="标题 3" xfId="45" builtinId="18"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="47" builtinId="31"/>
-    <cellStyle name="链接单元格" xfId="48" builtinId="24"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2617,19 +1999,19 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F351"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A335" workbookViewId="0">
-      <selection activeCell="D352" sqref="A350:D352"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="31.125" customWidth="1"/>
     <col min="2" max="2" width="18.75" customWidth="1"/>
@@ -2638,7 +2020,7 @@
     <col min="6" max="6" width="29.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="19.5" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2646,7 +2028,7 @@
       <c r="C1" s="2"/>
       <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -2660,7 +2042,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
         <v>5</v>
       </c>
@@ -2674,7 +2056,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
         <v>9</v>
       </c>
@@ -2686,7 +2068,7 @@
       </c>
       <c r="D4" s="8"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
         <v>12</v>
       </c>
@@ -2698,7 +2080,7 @@
       </c>
       <c r="D5" s="8"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
         <v>14</v>
       </c>
@@ -2710,7 +2092,7 @@
       </c>
       <c r="D6" s="8"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="6" t="s">
         <v>16</v>
       </c>
@@ -2722,7 +2104,7 @@
       </c>
       <c r="D7" s="8"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
         <v>19</v>
       </c>
@@ -2734,7 +2116,7 @@
       </c>
       <c r="D8" s="8"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="6" t="s">
         <v>22</v>
       </c>
@@ -2748,7 +2130,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="6" t="s">
         <v>26</v>
       </c>
@@ -2760,7 +2142,7 @@
       </c>
       <c r="D10" s="8"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="6" t="s">
         <v>28</v>
       </c>
@@ -2774,7 +2156,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" s="6" t="s">
         <v>31</v>
       </c>
@@ -2788,7 +2170,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="6" t="s">
         <v>34</v>
       </c>
@@ -2802,7 +2184,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" ht="19.5" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="10" t="s">
         <v>36</v>
       </c>
@@ -2816,9 +2198,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" ht="19.5"/>
-    <row r="16" ht="19.5"/>
-    <row r="17" ht="19.5" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" s="13" t="s">
         <v>38</v>
       </c>
@@ -2826,7 +2206,7 @@
       <c r="C17" s="14"/>
       <c r="D17" s="15"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" s="4" t="s">
         <v>1</v>
       </c>
@@ -2840,7 +2220,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" s="4" t="s">
         <v>39</v>
       </c>
@@ -2851,7 +2231,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" s="4" t="s">
         <v>42</v>
       </c>
@@ -2862,7 +2242,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" s="4" t="s">
         <v>44</v>
       </c>
@@ -2873,7 +2253,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22" s="4" t="s">
         <v>46</v>
       </c>
@@ -2884,7 +2264,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23" s="4" t="s">
         <v>48</v>
       </c>
@@ -2895,7 +2275,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24" s="4" t="s">
         <v>50</v>
       </c>
@@ -2909,7 +2289,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" ht="17" customHeight="1" spans="1:4">
+    <row r="25" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="4" t="s">
         <v>54</v>
       </c>
@@ -2923,7 +2303,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="s">
         <v>57</v>
       </c>
@@ -2933,7 +2313,7 @@
       <c r="C26" s="16"/>
       <c r="D26" s="5"/>
     </row>
-    <row r="27" ht="19.5" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A27" s="17" t="s">
         <v>58</v>
       </c>
@@ -2947,9 +2327,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" ht="19.5"/>
-    <row r="29" ht="19.5"/>
-    <row r="30" ht="19.5" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A30" s="13" t="s">
         <v>62</v>
       </c>
@@ -2957,7 +2335,7 @@
       <c r="C30" s="14"/>
       <c r="D30" s="15"/>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A31" s="4" t="s">
         <v>1</v>
       </c>
@@ -2971,58 +2349,58 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A32" s="4"/>
       <c r="B32" t="s">
         <v>63</v>
       </c>
       <c r="D32" s="5"/>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A33" s="4"/>
       <c r="B33" t="s">
         <v>40</v>
       </c>
       <c r="D33" s="5"/>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A34" s="4"/>
       <c r="B34" t="s">
         <v>43</v>
       </c>
       <c r="D34" s="5"/>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A35" s="4"/>
       <c r="B35" t="s">
         <v>45</v>
       </c>
       <c r="D35" s="5"/>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A36" s="4"/>
       <c r="B36" t="s">
         <v>47</v>
       </c>
       <c r="D36" s="5"/>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A37" s="4"/>
       <c r="B37" t="s">
         <v>64</v>
       </c>
       <c r="D37" s="5"/>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A38" s="4"/>
       <c r="B38" t="s">
         <v>65</v>
       </c>
       <c r="D38" s="5"/>
     </row>
-    <row r="39" ht="19.5" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A39" s="17" t="s">
-        <v>66</v>
+        <v>331</v>
       </c>
       <c r="B39" s="18" t="s">
         <v>55</v>
@@ -3032,104 +2410,78 @@
       </c>
       <c r="D39" s="19"/>
     </row>
-    <row r="40" ht="19.5" spans="2:2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B40" s="16"/>
     </row>
-    <row r="41" ht="19.5"/>
-    <row r="42" ht="19.5" spans="1:4">
-      <c r="A42" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="B42" s="14"/>
-      <c r="C42" s="14"/>
-      <c r="D42" s="15"/>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B43" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="C43" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="4"/>
-      <c r="B44" t="s">
-        <v>68</v>
-      </c>
-      <c r="D44" s="5"/>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="4"/>
-      <c r="B45" t="s">
-        <v>40</v>
-      </c>
-      <c r="D45" s="5"/>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="4"/>
-      <c r="B46" t="s">
-        <v>43</v>
-      </c>
-      <c r="D46" s="5"/>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" s="4"/>
-      <c r="B47" t="s">
-        <v>45</v>
-      </c>
-      <c r="D47" s="5"/>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="4"/>
-      <c r="B48" t="s">
-        <v>47</v>
-      </c>
-      <c r="D48" s="5"/>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="4"/>
-      <c r="B49" t="s">
-        <v>64</v>
-      </c>
-      <c r="D49" s="5"/>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="A50" s="4"/>
-      <c r="B50" t="s">
-        <v>65</v>
-      </c>
-      <c r="D50" s="5"/>
-    </row>
-    <row r="51" ht="19.5" spans="1:4">
-      <c r="A51" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="B51" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="C51" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="D51" s="19"/>
-    </row>
-    <row r="52" ht="19.5"/>
-    <row r="53" ht="19.5"/>
-    <row r="54" ht="19.5" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A42" s="16"/>
+      <c r="B42" s="16"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="16"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A43" s="16"/>
+      <c r="B43" s="16"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="16"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A44" s="16"/>
+      <c r="B44" s="16"/>
+      <c r="C44" s="16"/>
+      <c r="D44" s="16"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A45" s="16"/>
+      <c r="B45" s="16"/>
+      <c r="C45" s="16"/>
+      <c r="D45" s="16"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A46" s="16"/>
+      <c r="B46" s="16"/>
+      <c r="C46" s="16"/>
+      <c r="D46" s="16"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A47" s="16"/>
+      <c r="B47" s="16"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A48" s="16"/>
+      <c r="B48" s="16"/>
+      <c r="C48" s="16"/>
+      <c r="D48" s="16"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A49" s="16"/>
+      <c r="B49" s="16"/>
+      <c r="C49" s="16"/>
+      <c r="D49" s="16"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A50" s="16"/>
+      <c r="B50" s="16"/>
+      <c r="C50" s="16"/>
+      <c r="D50" s="16"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A51" s="16"/>
+      <c r="B51" s="16"/>
+      <c r="C51" s="16"/>
+      <c r="D51" s="16"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A54" s="13" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B54" s="14"/>
       <c r="C54" s="14"/>
       <c r="D54" s="15"/>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A55" s="4" t="s">
         <v>1</v>
       </c>
@@ -3143,83 +2495,83 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A56" s="4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B56" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C56" t="s">
         <v>7</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A57" s="4"/>
       <c r="B57" t="s">
         <v>10</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A58" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B58" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C58" t="s">
         <v>11</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A59" s="4"/>
       <c r="B59" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A60" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B60" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C60" t="s">
         <v>18</v>
       </c>
       <c r="D60" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A61" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B61" t="s">
+        <v>80</v>
+      </c>
+      <c r="C61" t="s">
+        <v>81</v>
+      </c>
+      <c r="D61" s="20" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
-      <c r="A61" s="4" t="s">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A62" s="4" t="s">
         <v>83</v>
-      </c>
-      <c r="B61" t="s">
-        <v>84</v>
-      </c>
-      <c r="C61" t="s">
-        <v>85</v>
-      </c>
-      <c r="D61" s="20" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4">
-      <c r="A62" s="4" t="s">
-        <v>87</v>
       </c>
       <c r="B62" t="s">
         <v>20</v>
@@ -3229,9 +2581,9 @@
       </c>
       <c r="D62" s="5"/>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A63" s="4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B63" t="s">
         <v>23</v>
@@ -3241,9 +2593,9 @@
       </c>
       <c r="D63" s="5"/>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A64" s="4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B64" t="s">
         <v>27</v>
@@ -3253,29 +2605,27 @@
       </c>
       <c r="D64" s="5"/>
     </row>
-    <row r="65" ht="19.5" spans="1:4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A65" s="17" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B65" s="18" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C65" s="18" t="s">
         <v>18</v>
       </c>
       <c r="D65" s="19"/>
     </row>
-    <row r="66" ht="19.5"/>
-    <row r="67" ht="19.5"/>
-    <row r="68" ht="19.5" spans="1:4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A68" s="13" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B68" s="14"/>
       <c r="C68" s="14"/>
       <c r="D68" s="15"/>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A69" s="4" t="s">
         <v>1</v>
       </c>
@@ -3289,144 +2639,144 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A70" s="4"/>
       <c r="B70" t="s">
         <v>40</v>
       </c>
       <c r="D70" s="5"/>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A71" s="4"/>
       <c r="B71" t="s">
         <v>43</v>
       </c>
       <c r="D71" s="5"/>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A72" s="4"/>
       <c r="B72" t="s">
         <v>45</v>
       </c>
       <c r="D72" s="5"/>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A73" s="4"/>
       <c r="B73" t="s">
         <v>47</v>
       </c>
       <c r="D73" s="5"/>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A74" s="4"/>
       <c r="B74" t="s">
         <v>49</v>
       </c>
       <c r="D74" s="5"/>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A75" s="4"/>
       <c r="B75" t="s">
+        <v>89</v>
+      </c>
+      <c r="D75" s="20" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A76" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B76" t="s">
+        <v>92</v>
+      </c>
+      <c r="C76" t="s">
         <v>93</v>
       </c>
-      <c r="D75" s="20" t="s">
+      <c r="D76" s="20" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="76" spans="1:4">
-      <c r="A76" s="4" t="s">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A77" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B77" t="s">
         <v>96</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C77" t="s">
         <v>97</v>
       </c>
-      <c r="D76" s="20" t="s">
+      <c r="D77" s="20" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="77" spans="1:4">
-      <c r="A77" s="4" t="s">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A78" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B78" t="s">
         <v>100</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C78" t="s">
+        <v>97</v>
+      </c>
+      <c r="D78" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="D77" s="20" t="s">
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A79" s="4" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="78" spans="1:4">
-      <c r="A78" s="4" t="s">
+      <c r="B79" t="s">
         <v>103</v>
       </c>
-      <c r="B78" t="s">
+      <c r="C79" t="s">
+        <v>97</v>
+      </c>
+      <c r="D79" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="C78" t="s">
-        <v>101</v>
-      </c>
-      <c r="D78" s="20" t="s">
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A80" s="4" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="79" spans="1:4">
-      <c r="A79" s="4" t="s">
+      <c r="B80" t="s">
         <v>106</v>
       </c>
-      <c r="B79" t="s">
+      <c r="C80" t="s">
+        <v>97</v>
+      </c>
+      <c r="D80" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="C79" t="s">
-        <v>101</v>
-      </c>
-      <c r="D79" s="20" t="s">
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A81" s="4" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="80" spans="1:4">
-      <c r="A80" s="4" t="s">
+      <c r="B81" t="s">
         <v>109</v>
       </c>
-      <c r="B80" t="s">
+      <c r="C81" t="s">
+        <v>97</v>
+      </c>
+      <c r="D81" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="C80" t="s">
-        <v>101</v>
-      </c>
-      <c r="D80" s="20" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4">
-      <c r="A81" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="B81" t="s">
-        <v>113</v>
-      </c>
-      <c r="C81" t="s">
-        <v>101</v>
-      </c>
-      <c r="D81" s="20" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4">
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A82" s="4"/>
       <c r="B82" t="s">
         <v>6</v>
       </c>
       <c r="D82" s="5"/>
     </row>
-    <row r="83" ht="19.5" spans="1:4">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A83" s="17" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B83" s="18" t="s">
         <v>20</v>
@@ -3435,20 +2785,18 @@
         <v>21</v>
       </c>
       <c r="D83" s="19" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="84" ht="19.5"/>
-    <row r="85" ht="19.5"/>
-    <row r="86" ht="19.5" spans="1:4">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A86" s="13" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B86" s="14"/>
       <c r="C86" s="14"/>
       <c r="D86" s="15"/>
     </row>
-    <row r="87" spans="1:4">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A87" s="4" t="s">
         <v>1</v>
       </c>
@@ -3462,79 +2810,79 @@
         <v>4</v>
       </c>
     </row>
-    <row r="88" spans="1:4">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A88" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B88" t="s">
+        <v>115</v>
+      </c>
+      <c r="C88" t="s">
+        <v>93</v>
+      </c>
+      <c r="D88" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A89" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B89" t="s">
         <v>118</v>
       </c>
-      <c r="B88" t="s">
+      <c r="C89" t="s">
+        <v>93</v>
+      </c>
+      <c r="D89" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="C88" t="s">
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A90" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B90" t="s">
+        <v>121</v>
+      </c>
+      <c r="C90" t="s">
         <v>97</v>
       </c>
-      <c r="D88" s="5" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4">
-      <c r="A89" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="B89" t="s">
+      <c r="D90" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="C89" t="s">
-        <v>97</v>
-      </c>
-      <c r="D89" s="20" t="s">
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A91" s="4" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="90" spans="1:4">
-      <c r="A90" s="4" t="s">
+      <c r="B91" t="s">
         <v>124</v>
       </c>
-      <c r="B90" t="s">
+      <c r="C91" t="s">
         <v>125</v>
       </c>
-      <c r="C90" t="s">
-        <v>101</v>
-      </c>
-      <c r="D90" s="5" t="s">
+      <c r="D91" s="5" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="91" spans="1:4">
-      <c r="A91" s="4" t="s">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A92" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B92" t="s">
         <v>128</v>
-      </c>
-      <c r="C91" t="s">
-        <v>129</v>
-      </c>
-      <c r="D91" s="5" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4">
-      <c r="A92" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="B92" t="s">
-        <v>132</v>
       </c>
       <c r="C92" t="s">
         <v>60</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="93" ht="19.5" spans="1:4">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A93" s="17" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B93" s="18" t="s">
         <v>20</v>
@@ -3543,20 +2891,18 @@
         <v>21</v>
       </c>
       <c r="D93" s="19" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="94" ht="19.5"/>
-    <row r="95" ht="19.5"/>
-    <row r="96" ht="19.5" spans="1:4">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A96" s="13" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B96" s="14"/>
       <c r="C96" s="14"/>
       <c r="D96" s="15"/>
     </row>
-    <row r="97" spans="1:4">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A97" s="4" t="s">
         <v>1</v>
       </c>
@@ -3570,88 +2916,88 @@
         <v>4</v>
       </c>
     </row>
-    <row r="98" spans="1:4">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A98" s="4" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B98" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C98" t="s">
         <v>7</v>
       </c>
       <c r="D98" s="5" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A99" s="4"/>
       <c r="B99" t="s">
         <v>10</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A100" s="4"/>
       <c r="B100" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D100" s="5"/>
     </row>
-    <row r="101" spans="1:4">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A101" s="4" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B101" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C101" t="s">
         <v>18</v>
       </c>
       <c r="D101" s="5" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A102" s="4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B102" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C102" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D102" s="20" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A103" s="4"/>
       <c r="B103" t="s">
         <v>20</v>
       </c>
       <c r="D103" s="5"/>
     </row>
-    <row r="104" spans="1:4">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A104" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B104" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C104" t="s">
         <v>7</v>
       </c>
       <c r="D104" s="5" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A105" s="4" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B105" t="s">
         <v>23</v>
@@ -3660,21 +3006,21 @@
         <v>24</v>
       </c>
       <c r="D105" s="5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A106" s="4" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B106" t="s">
         <v>27</v>
       </c>
       <c r="D106" s="5"/>
     </row>
-    <row r="107" ht="19.5" spans="1:4">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A107" s="17" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B107" s="18" t="s">
         <v>29</v>
@@ -3682,13 +3028,12 @@
       <c r="C107" s="18"/>
       <c r="D107" s="19"/>
     </row>
-    <row r="108" ht="19.5"/>
-    <row r="109" ht="19.5" spans="6:6">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.15">
       <c r="F109" s="18"/>
     </row>
-    <row r="110" ht="19.5" spans="1:6">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A110" s="13" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B110" s="14"/>
       <c r="C110" s="14"/>
@@ -3696,7 +3041,7 @@
       <c r="E110" s="14"/>
       <c r="F110" s="5"/>
     </row>
-    <row r="111" spans="1:6">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A111" s="4" t="s">
         <v>1</v>
       </c>
@@ -3712,7 +3057,7 @@
       <c r="E111" s="16"/>
       <c r="F111" s="5"/>
     </row>
-    <row r="112" spans="1:6">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A112" s="4"/>
       <c r="B112" t="s">
         <v>40</v>
@@ -3721,7 +3066,7 @@
       <c r="E112" s="16"/>
       <c r="F112" s="5"/>
     </row>
-    <row r="113" spans="1:6">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A113" s="4"/>
       <c r="B113" t="s">
         <v>43</v>
@@ -3730,7 +3075,7 @@
       <c r="E113" s="16"/>
       <c r="F113" s="5"/>
     </row>
-    <row r="114" spans="1:6">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A114" s="4"/>
       <c r="B114" t="s">
         <v>45</v>
@@ -3739,7 +3084,7 @@
       <c r="E114" s="16"/>
       <c r="F114" s="5"/>
     </row>
-    <row r="115" spans="1:6">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A115" s="4"/>
       <c r="B115" t="s">
         <v>47</v>
@@ -3748,7 +3093,7 @@
       <c r="E115" s="16"/>
       <c r="F115" s="5"/>
     </row>
-    <row r="116" spans="1:6">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A116" s="4"/>
       <c r="B116" t="s">
         <v>49</v>
@@ -3757,139 +3102,139 @@
       <c r="E116" s="16"/>
       <c r="F116" s="5"/>
     </row>
-    <row r="117" spans="1:6">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A117" s="4"/>
       <c r="B117" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D117" s="21" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="E117" s="16"/>
       <c r="F117" s="5" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A118" s="4" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B118" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C118" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D118" s="21" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E118" s="16"/>
       <c r="F118" s="5" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A119" s="4" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B119" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C119" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D119" s="21" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E119" s="16"/>
       <c r="F119" s="5" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A120" s="4" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B120" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C120" t="s">
+        <v>97</v>
+      </c>
+      <c r="D120" s="21" t="s">
         <v>101</v>
-      </c>
-      <c r="D120" s="21" t="s">
-        <v>105</v>
       </c>
       <c r="E120" s="16"/>
       <c r="F120" s="5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A121" s="4" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="121" spans="1:6">
-      <c r="A121" s="4" t="s">
-        <v>160</v>
-      </c>
       <c r="B121" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C121" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D121" s="21" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E121" s="16"/>
       <c r="F121" s="5" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A122" s="4" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B122" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C122" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D122" s="21" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E122" s="16"/>
       <c r="F122" s="5" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A123" s="4" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B123" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C123" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D123" s="21" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E123" s="16"/>
       <c r="F123" s="5"/>
     </row>
-    <row r="124" spans="1:6">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A124" s="4"/>
       <c r="B124" t="s">
         <v>6</v>
       </c>
       <c r="D124" s="16" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E124" s="16"/>
       <c r="F124" s="5"/>
     </row>
-    <row r="125" ht="19.5" spans="1:6">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A125" s="17" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B125" s="18" t="s">
         <v>20</v>
@@ -3898,23 +3243,21 @@
         <v>21</v>
       </c>
       <c r="D125" s="18" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E125" s="18"/>
       <c r="F125" s="19"/>
     </row>
-    <row r="126" ht="19.5"/>
-    <row r="127" ht="19.5"/>
-    <row r="128" ht="19.5" spans="1:5">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A128" s="13" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B128" s="14"/>
       <c r="C128" s="14"/>
       <c r="D128" s="14"/>
       <c r="E128" s="15"/>
     </row>
-    <row r="129" spans="1:5">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A129" s="4" t="s">
         <v>1</v>
       </c>
@@ -3929,99 +3272,99 @@
       </c>
       <c r="E129" s="5"/>
     </row>
-    <row r="130" spans="1:5">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A130" s="4" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B130" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C130" t="s">
         <v>7</v>
       </c>
       <c r="D130" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E130" s="5"/>
     </row>
-    <row r="131" spans="1:5">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A131" s="4"/>
       <c r="B131" t="s">
         <v>10</v>
       </c>
       <c r="D131" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E131" s="5"/>
     </row>
-    <row r="132" spans="1:5">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A132" s="4" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B132" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C132" t="s">
         <v>24</v>
       </c>
       <c r="D132" s="22" t="s">
+        <v>168</v>
+      </c>
+      <c r="E132" s="5"/>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A133" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="B133" t="s">
+        <v>170</v>
+      </c>
+      <c r="C133" t="s">
+        <v>171</v>
+      </c>
+      <c r="D133" t="s">
         <v>172</v>
       </c>
-      <c r="E132" s="5"/>
-    </row>
-    <row r="133" spans="1:5">
-      <c r="A133" s="4" t="s">
+      <c r="E133" s="5"/>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A134" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="B133" t="s">
-        <v>174</v>
-      </c>
-      <c r="C133" t="s">
-        <v>175</v>
-      </c>
-      <c r="D133" t="s">
-        <v>176</v>
-      </c>
-      <c r="E133" s="5"/>
-    </row>
-    <row r="134" spans="1:5">
-      <c r="A134" s="4" t="s">
-        <v>177</v>
-      </c>
       <c r="B134" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C134" t="s">
         <v>18</v>
       </c>
       <c r="D134" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E134" s="5"/>
     </row>
-    <row r="135" spans="1:5">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A135" s="4" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B135" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C135" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D135" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E135" s="5"/>
     </row>
-    <row r="136" spans="1:5">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A136" s="4"/>
       <c r="B136" t="s">
         <v>20</v>
       </c>
       <c r="E136" s="5"/>
     </row>
-    <row r="137" spans="1:5">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A137" s="4"/>
       <c r="B137" t="s">
         <v>23</v>
@@ -4030,18 +3373,18 @@
         <v>24</v>
       </c>
       <c r="D137" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E137" s="5"/>
     </row>
-    <row r="138" spans="1:5">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A138" s="4"/>
       <c r="B138" t="s">
         <v>27</v>
       </c>
       <c r="E138" s="5"/>
     </row>
-    <row r="139" ht="19.5" spans="1:5">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A139" s="17"/>
       <c r="B139" s="18" t="s">
         <v>29</v>
@@ -4050,17 +3393,15 @@
       <c r="D139" s="18"/>
       <c r="E139" s="19"/>
     </row>
-    <row r="140" ht="19.5"/>
-    <row r="141" ht="19.5"/>
-    <row r="142" ht="19.5" spans="1:4">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A142" s="13" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B142" s="14"/>
       <c r="C142" s="14"/>
       <c r="D142" s="15"/>
     </row>
-    <row r="143" spans="1:4">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A143" s="4" t="s">
         <v>1</v>
       </c>
@@ -4074,140 +3415,140 @@
         <v>4</v>
       </c>
     </row>
-    <row r="144" spans="1:4">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A144" s="4"/>
       <c r="B144" t="s">
         <v>40</v>
       </c>
       <c r="D144" s="5"/>
     </row>
-    <row r="145" spans="1:4">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A145" s="4"/>
       <c r="B145" t="s">
         <v>43</v>
       </c>
       <c r="D145" s="5"/>
     </row>
-    <row r="146" spans="1:4">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A146" s="4"/>
       <c r="B146" t="s">
         <v>45</v>
       </c>
       <c r="D146" s="5"/>
     </row>
-    <row r="147" spans="1:4">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A147" s="4"/>
       <c r="B147" t="s">
         <v>47</v>
       </c>
       <c r="D147" s="5"/>
     </row>
-    <row r="148" spans="1:4">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A148" s="4"/>
       <c r="B148" t="s">
         <v>49</v>
       </c>
       <c r="D148" s="5"/>
     </row>
-    <row r="149" spans="1:4">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A149" s="4"/>
       <c r="B149" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C149" t="s">
         <v>52</v>
       </c>
       <c r="D149" s="20" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A150" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="B150" t="s">
+        <v>92</v>
+      </c>
+      <c r="C150" t="s">
+        <v>93</v>
+      </c>
+      <c r="D150" s="20" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A151" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B151" t="s">
+        <v>96</v>
+      </c>
+      <c r="C151" t="s">
+        <v>97</v>
+      </c>
+      <c r="D151" s="20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A152" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B152" t="s">
+        <v>100</v>
+      </c>
+      <c r="C152" t="s">
+        <v>97</v>
+      </c>
+      <c r="D152" s="20" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A153" s="4" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="150" spans="1:4">
-      <c r="A150" s="4" t="s">
+      <c r="B153" t="s">
+        <v>103</v>
+      </c>
+      <c r="C153" t="s">
+        <v>97</v>
+      </c>
+      <c r="D153" s="20" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A154" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="B150" t="s">
-        <v>96</v>
-      </c>
-      <c r="C150" t="s">
+      <c r="B154" t="s">
+        <v>106</v>
+      </c>
+      <c r="C154" t="s">
         <v>97</v>
       </c>
-      <c r="D150" s="20" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4">
-      <c r="A151" s="4" t="s">
+      <c r="D154" s="20" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A155" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="B151" t="s">
-        <v>100</v>
-      </c>
-      <c r="C151" t="s">
-        <v>101</v>
-      </c>
-      <c r="D151" s="20" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4">
-      <c r="A152" s="4" t="s">
+      <c r="B155" t="s">
+        <v>109</v>
+      </c>
+      <c r="C155" t="s">
+        <v>97</v>
+      </c>
+      <c r="D155" s="20" t="s">
         <v>186</v>
       </c>
-      <c r="B152" t="s">
-        <v>104</v>
-      </c>
-      <c r="C152" t="s">
-        <v>101</v>
-      </c>
-      <c r="D152" s="20" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4">
-      <c r="A153" s="4" t="s">
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A156" s="17" t="s">
         <v>187</v>
-      </c>
-      <c r="B153" t="s">
-        <v>107</v>
-      </c>
-      <c r="C153" t="s">
-        <v>101</v>
-      </c>
-      <c r="D153" s="20" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4">
-      <c r="A154" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="B154" t="s">
-        <v>110</v>
-      </c>
-      <c r="C154" t="s">
-        <v>101</v>
-      </c>
-      <c r="D154" s="20" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4">
-      <c r="A155" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="B155" t="s">
-        <v>113</v>
-      </c>
-      <c r="C155" t="s">
-        <v>101</v>
-      </c>
-      <c r="D155" s="20" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="156" ht="19.5" spans="1:4">
-      <c r="A156" s="17" t="s">
-        <v>191</v>
       </c>
       <c r="B156" s="18" t="s">
         <v>20</v>
@@ -4216,20 +3557,18 @@
         <v>21</v>
       </c>
       <c r="D156" s="19" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="157" ht="19.5"/>
-    <row r="158" ht="19.5"/>
-    <row r="159" ht="19.5" spans="1:4">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A159" s="13" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B159" s="14"/>
       <c r="C159" s="14"/>
       <c r="D159" s="15"/>
     </row>
-    <row r="160" spans="1:4">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A160" s="4" t="s">
         <v>1</v>
       </c>
@@ -4243,74 +3582,74 @@
         <v>4</v>
       </c>
     </row>
-    <row r="161" spans="1:4">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A161" s="4" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B161" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C161" t="s">
         <v>7</v>
       </c>
       <c r="D161" s="5" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="162" spans="1:4">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A162" s="4"/>
       <c r="B162" t="s">
         <v>10</v>
       </c>
       <c r="D162" s="5" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="163" spans="1:4">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A163" s="4" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B163" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C163" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D163" s="5" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="164" spans="1:4">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A164" s="4" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B164" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C164" t="s">
         <v>11</v>
       </c>
       <c r="D164" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="165" spans="1:4">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A165" s="4" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B165" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C165" t="s">
         <v>18</v>
       </c>
       <c r="D165" s="5" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="166" spans="1:4">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A166" s="4" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B166" t="s">
         <v>15</v>
@@ -4319,19 +3658,19 @@
         <v>11</v>
       </c>
       <c r="D166" s="5" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="167" spans="1:4">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A167" s="4"/>
       <c r="B167" t="s">
         <v>20</v>
       </c>
       <c r="D167" s="5" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="168" spans="1:4">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A168" s="4"/>
       <c r="B168" t="s">
         <v>23</v>
@@ -4340,17 +3679,17 @@
         <v>24</v>
       </c>
       <c r="D168" s="5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="169" spans="1:4">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A169" s="4"/>
       <c r="B169" t="s">
         <v>27</v>
       </c>
       <c r="D169" s="5"/>
     </row>
-    <row r="170" ht="19.5" spans="1:4">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A170" s="17"/>
       <c r="B170" s="18" t="s">
         <v>29</v>
@@ -4360,17 +3699,15 @@
       </c>
       <c r="D170" s="19"/>
     </row>
-    <row r="171" ht="19.5"/>
-    <row r="172" ht="19.5"/>
-    <row r="173" ht="19.5" spans="1:4">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A173" s="13" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B173" s="14"/>
       <c r="C173" s="14"/>
       <c r="D173" s="15"/>
     </row>
-    <row r="174" spans="1:4">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A174" s="4" t="s">
         <v>1</v>
       </c>
@@ -4384,9 +3721,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="175" spans="1:4">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A175" s="4" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B175" t="s">
         <v>40</v>
@@ -4395,7 +3732,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="176" spans="1:4">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A176" s="4"/>
       <c r="B176" t="s">
         <v>43</v>
@@ -4404,7 +3741,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="177" spans="1:4">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A177" s="4"/>
       <c r="B177" t="s">
         <v>45</v>
@@ -4413,7 +3750,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="178" spans="1:4">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A178" s="4"/>
       <c r="B178" t="s">
         <v>47</v>
@@ -4422,7 +3759,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="179" spans="1:4">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A179" s="4"/>
       <c r="B179" t="s">
         <v>49</v>
@@ -4431,23 +3768,23 @@
         <v>41</v>
       </c>
     </row>
-    <row r="180" spans="1:4">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A180" s="4" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B180" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C180" t="s">
         <v>52</v>
       </c>
       <c r="D180" s="20" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="181" spans="1:4">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A181" s="4" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B181" t="s">
         <v>55</v>
@@ -4456,32 +3793,30 @@
         <v>52</v>
       </c>
       <c r="D181" s="5" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="182" ht="19.5" spans="1:4">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A182" s="17"/>
       <c r="B182" s="18" t="s">
         <v>20</v>
       </c>
       <c r="C182" s="18"/>
       <c r="D182" s="19" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="183" ht="19.5"/>
-    <row r="184" ht="19.5"/>
-    <row r="185" ht="21.75" spans="1:4">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A185" s="13" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B185" s="23" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C185" s="14"/>
       <c r="D185" s="15"/>
     </row>
-    <row r="186" spans="1:4">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A186" s="4" t="s">
         <v>1</v>
       </c>
@@ -4495,97 +3830,97 @@
         <v>4</v>
       </c>
     </row>
-    <row r="187" spans="1:4">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A187" s="4" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B187" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C187" t="s">
         <v>7</v>
       </c>
       <c r="D187" s="5" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="188" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A188" s="4"/>
       <c r="B188" t="s">
         <v>10</v>
       </c>
       <c r="D188" s="5" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="189" spans="1:4">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A189" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B189" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C189" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D189" s="5" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="190" spans="1:4">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A190" s="4" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="B190" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C190" t="s">
         <v>11</v>
       </c>
       <c r="D190" s="5" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="191" spans="1:4">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A191" s="4" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B191" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C191" t="s">
         <v>18</v>
       </c>
       <c r="D191" s="5" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="192" spans="1:4">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A192" s="4"/>
       <c r="B192" t="s">
         <v>20</v>
       </c>
       <c r="D192" s="5" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="193" spans="1:4">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A193" s="4" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B193" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C193" t="s">
         <v>7</v>
       </c>
       <c r="D193" s="5" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="194" spans="1:4">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A194" s="4" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B194" t="s">
         <v>23</v>
@@ -4594,39 +3929,37 @@
         <v>24</v>
       </c>
       <c r="D194" s="24" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="195" spans="1:4">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A195" s="4"/>
       <c r="B195" t="s">
         <v>27</v>
       </c>
       <c r="D195" s="24" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="196" ht="19.5" spans="1:4">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A196" s="17"/>
       <c r="B196" s="18" t="s">
         <v>29</v>
       </c>
       <c r="C196" s="18"/>
       <c r="D196" s="19" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="197" ht="19.5"/>
-    <row r="198" ht="19.5"/>
-    <row r="199" ht="19.5" spans="1:4">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A199" s="13" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B199" s="14"/>
       <c r="C199" s="14"/>
       <c r="D199" s="15"/>
     </row>
-    <row r="200" spans="1:4">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A200" s="4" t="s">
         <v>1</v>
       </c>
@@ -4640,81 +3973,79 @@
         <v>4</v>
       </c>
     </row>
-    <row r="201" spans="1:4">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A201" s="4"/>
       <c r="B201" t="s">
         <v>40</v>
       </c>
       <c r="D201" s="5" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="202" spans="1:4">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A202" s="4"/>
       <c r="B202" t="s">
         <v>43</v>
       </c>
       <c r="D202" s="5" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="203" spans="1:4">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A203" s="4"/>
       <c r="B203" t="s">
         <v>45</v>
       </c>
       <c r="D203" s="5" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="204" spans="1:4">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A204" s="4"/>
       <c r="B204" t="s">
         <v>47</v>
       </c>
       <c r="D204" s="5" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="205" spans="1:4">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A205" s="4"/>
       <c r="B205" t="s">
         <v>49</v>
       </c>
       <c r="D205" s="5" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="206" spans="1:4">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A206" s="4"/>
       <c r="B206" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D206" s="5" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="207" ht="19.5" spans="1:4">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A207" s="17"/>
       <c r="B207" s="18" t="s">
         <v>20</v>
       </c>
       <c r="C207" s="18"/>
       <c r="D207" s="19" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="208" ht="19.5"/>
-    <row r="209" ht="19.5"/>
-    <row r="210" ht="19.5" spans="1:4">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A210" s="13" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B210" s="14"/>
       <c r="C210" s="14"/>
       <c r="D210" s="15"/>
     </row>
-    <row r="211" spans="1:4">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A211" s="4" t="s">
         <v>1</v>
       </c>
@@ -4728,95 +4059,95 @@
         <v>4</v>
       </c>
     </row>
-    <row r="212" spans="1:4">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A212" s="4" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B212" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C212" t="s">
         <v>7</v>
       </c>
       <c r="D212" s="5" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="213" spans="1:4">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A213" s="4"/>
       <c r="B213" t="s">
         <v>10</v>
       </c>
       <c r="D213" s="5" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="214" spans="1:4">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A214" s="4" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B214" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C214" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D214" s="5" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="215" spans="1:4">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A215" s="4" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B215" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C215" t="s">
         <v>11</v>
       </c>
       <c r="D215" s="5" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="216" spans="1:4">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A216" s="4" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="B216" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C216" t="s">
         <v>18</v>
       </c>
       <c r="D216" s="5" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="217" spans="1:4">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A217" s="4"/>
       <c r="B217" t="s">
         <v>20</v>
       </c>
       <c r="D217" s="24" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="218" spans="1:4">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A218" s="4" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B218" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C218" t="s">
         <v>7</v>
       </c>
       <c r="D218" s="5" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="219" spans="1:4">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A219" s="4"/>
       <c r="B219" t="s">
         <v>23</v>
@@ -4825,17 +4156,17 @@
         <v>24</v>
       </c>
       <c r="D219" s="24" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="220" spans="1:4">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A220" s="4"/>
       <c r="B220" t="s">
         <v>27</v>
       </c>
       <c r="D220" s="5"/>
     </row>
-    <row r="221" ht="19.5" spans="1:4">
+    <row r="221" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A221" s="17"/>
       <c r="B221" s="18" t="s">
         <v>29</v>
@@ -4843,17 +4174,15 @@
       <c r="C221" s="18"/>
       <c r="D221" s="19"/>
     </row>
-    <row r="222" ht="19.5"/>
-    <row r="223" ht="19.5"/>
-    <row r="224" ht="19.5" spans="1:4">
+    <row r="224" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A224" s="13" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B224" s="14"/>
       <c r="C224" s="14"/>
       <c r="D224" s="15"/>
     </row>
-    <row r="225" spans="1:4">
+    <row r="225" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A225" s="4" t="s">
         <v>1</v>
       </c>
@@ -4867,49 +4196,49 @@
         <v>4</v>
       </c>
     </row>
-    <row r="226" spans="1:4">
+    <row r="226" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A226" s="4"/>
       <c r="B226" t="s">
         <v>40</v>
       </c>
       <c r="D226" s="5"/>
     </row>
-    <row r="227" spans="1:4">
+    <row r="227" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A227" s="4"/>
       <c r="B227" t="s">
         <v>43</v>
       </c>
       <c r="D227" s="5"/>
     </row>
-    <row r="228" spans="1:4">
+    <row r="228" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A228" s="4"/>
       <c r="B228" t="s">
         <v>45</v>
       </c>
       <c r="D228" s="5"/>
     </row>
-    <row r="229" spans="1:4">
+    <row r="229" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A229" s="4"/>
       <c r="B229" t="s">
         <v>47</v>
       </c>
       <c r="D229" s="5"/>
     </row>
-    <row r="230" spans="1:4">
+    <row r="230" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A230" s="4"/>
       <c r="B230" t="s">
         <v>49</v>
       </c>
       <c r="D230" s="5"/>
     </row>
-    <row r="231" spans="1:4">
+    <row r="231" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A231" s="4"/>
       <c r="B231" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D231" s="5"/>
     </row>
-    <row r="232" ht="19.5" spans="1:4">
+    <row r="232" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A232" s="17"/>
       <c r="B232" s="18" t="s">
         <v>20</v>
@@ -4917,17 +4246,15 @@
       <c r="C232" s="18"/>
       <c r="D232" s="19"/>
     </row>
-    <row r="233" ht="19.5"/>
-    <row r="247" ht="19.5"/>
-    <row r="248" ht="19.5" spans="1:4">
+    <row r="248" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A248" s="13" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B248" s="14"/>
       <c r="C248" s="14"/>
       <c r="D248" s="15"/>
     </row>
-    <row r="249" spans="1:4">
+    <row r="249" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A249" s="4" t="s">
         <v>1</v>
       </c>
@@ -4941,74 +4268,74 @@
         <v>4</v>
       </c>
     </row>
-    <row r="250" spans="1:4">
+    <row r="250" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A250" s="4" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B250" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C250" t="s">
         <v>7</v>
       </c>
       <c r="D250" s="5" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="251" spans="1:4">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A251" s="4"/>
       <c r="B251" t="s">
         <v>10</v>
       </c>
       <c r="D251" s="5" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="252" spans="1:4">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A252" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="B252" t="s">
+        <v>249</v>
+      </c>
+      <c r="C252" t="s">
+        <v>171</v>
+      </c>
+      <c r="D252" s="5" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A253" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="B253" t="s">
         <v>252</v>
       </c>
-      <c r="B252" t="s">
+      <c r="C253" t="s">
+        <v>171</v>
+      </c>
+      <c r="D253" s="20" t="s">
         <v>253</v>
       </c>
-      <c r="C252" t="s">
-        <v>175</v>
-      </c>
-      <c r="D252" s="5" t="s">
+    </row>
+    <row r="254" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A254" s="4" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="253" spans="1:4">
-      <c r="A253" s="4" t="s">
+      <c r="B254" t="s">
         <v>255</v>
-      </c>
-      <c r="B253" t="s">
-        <v>256</v>
-      </c>
-      <c r="C253" t="s">
-        <v>175</v>
-      </c>
-      <c r="D253" s="20" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="254" spans="1:4">
-      <c r="A254" s="4" t="s">
-        <v>258</v>
-      </c>
-      <c r="B254" t="s">
-        <v>259</v>
       </c>
       <c r="C254" t="s">
         <v>18</v>
       </c>
       <c r="D254" s="5" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="255" spans="1:4">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A255" s="4" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="B255" t="s">
         <v>15</v>
@@ -5017,12 +4344,12 @@
         <v>11</v>
       </c>
       <c r="D255" s="5" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="256" spans="1:4">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A256" s="4" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B256" t="s">
         <v>23</v>
@@ -5031,17 +4358,17 @@
         <v>24</v>
       </c>
       <c r="D256" s="5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="257" spans="1:4">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A257" s="4"/>
       <c r="B257" t="s">
         <v>27</v>
       </c>
       <c r="D257" s="5"/>
     </row>
-    <row r="258" ht="19.5" spans="1:4">
+    <row r="258" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A258" s="17"/>
       <c r="B258" s="18" t="s">
         <v>29</v>
@@ -5049,17 +4376,15 @@
       <c r="C258" s="18"/>
       <c r="D258" s="19"/>
     </row>
-    <row r="259" ht="19.5"/>
-    <row r="260" ht="19.5"/>
-    <row r="261" ht="19.5" spans="1:4">
+    <row r="261" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A261" s="13" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B261" s="14"/>
       <c r="C261" s="14"/>
       <c r="D261" s="15"/>
     </row>
-    <row r="262" spans="1:4">
+    <row r="262" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A262" s="4" t="s">
         <v>1</v>
       </c>
@@ -5073,68 +4398,68 @@
         <v>4</v>
       </c>
     </row>
-    <row r="263" spans="1:4">
+    <row r="263" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A263" s="4"/>
       <c r="B263" t="s">
         <v>40</v>
       </c>
       <c r="D263" s="24" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="264" spans="1:4">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="264" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A264" s="4"/>
       <c r="B264" t="s">
         <v>43</v>
       </c>
       <c r="D264" s="24" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="265" spans="1:4">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A265" s="4"/>
       <c r="B265" t="s">
         <v>45</v>
       </c>
       <c r="D265" s="24" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="266" spans="1:4">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A266" s="4"/>
       <c r="B266" t="s">
         <v>47</v>
       </c>
       <c r="D266" s="24" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="267" spans="1:4">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A267" s="4"/>
       <c r="B267" t="s">
         <v>49</v>
       </c>
       <c r="D267" s="24" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="268" spans="1:4">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="268" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A268" s="4" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="B268" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="C268" t="s">
         <v>52</v>
       </c>
       <c r="D268" s="5" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="269" spans="1:4">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="269" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A269" s="4" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="B269" t="s">
         <v>55</v>
@@ -5143,10 +4468,10 @@
         <v>52</v>
       </c>
       <c r="D269" s="24" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="270" ht="19.5" spans="1:4">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="270" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A270" s="17"/>
       <c r="B270" s="18" t="s">
         <v>20</v>
@@ -5154,17 +4479,15 @@
       <c r="C270" s="18"/>
       <c r="D270" s="19"/>
     </row>
-    <row r="271" ht="19.5"/>
-    <row r="272" ht="19.5"/>
-    <row r="273" ht="19.5" spans="1:4">
+    <row r="273" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A273" s="13" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B273" s="14"/>
       <c r="C273" s="14"/>
       <c r="D273" s="15"/>
     </row>
-    <row r="274" spans="1:4">
+    <row r="274" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A274" s="4" t="s">
         <v>1</v>
       </c>
@@ -5178,72 +4501,72 @@
         <v>4</v>
       </c>
     </row>
-    <row r="275" spans="1:4">
+    <row r="275" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A275" s="4" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="B275" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C275" t="s">
         <v>7</v>
       </c>
       <c r="D275" s="5" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="276" ht="19" customHeight="1" spans="1:4">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="276" spans="1:4" ht="18.95" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A276" s="4"/>
       <c r="B276" t="s">
         <v>10</v>
       </c>
       <c r="D276" s="5" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="277" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A277" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="B277" t="s">
+        <v>249</v>
+      </c>
+      <c r="C277" t="s">
+        <v>171</v>
+      </c>
+      <c r="D277" s="5" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="278" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A278" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="B278" t="s">
+        <v>252</v>
+      </c>
+      <c r="C278" t="s">
+        <v>171</v>
+      </c>
+      <c r="D278" s="5" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="279" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A279" s="4" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="277" spans="1:4">
-      <c r="A277" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="B277" t="s">
-        <v>253</v>
-      </c>
-      <c r="C277" t="s">
-        <v>175</v>
-      </c>
-      <c r="D277" s="5" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="278" spans="1:4">
-      <c r="A278" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="B278" t="s">
-        <v>256</v>
-      </c>
-      <c r="C278" t="s">
-        <v>175</v>
-      </c>
-      <c r="D278" s="5" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="279" spans="1:4">
-      <c r="A279" s="4" t="s">
-        <v>277</v>
-      </c>
       <c r="B279" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C279" t="s">
         <v>18</v>
       </c>
       <c r="D279" s="5" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="280" spans="1:4">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="280" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A280" s="4"/>
       <c r="B280" t="s">
         <v>23</v>
@@ -5252,41 +4575,39 @@
         <v>24</v>
       </c>
       <c r="D280" s="5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="281" spans="1:4">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="281" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A281" s="4"/>
       <c r="B281" t="s">
         <v>27</v>
       </c>
       <c r="D281" s="5" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="282" ht="19.5" spans="1:4">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="282" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A282" s="17" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="B282" s="18" t="s">
         <v>29</v>
       </c>
       <c r="C282" s="18"/>
       <c r="D282" s="19" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="283" ht="19.5"/>
-    <row r="284" ht="19.5"/>
-    <row r="285" ht="19.5" spans="1:4">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="285" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A285" s="13" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="B285" s="14"/>
       <c r="C285" s="14"/>
       <c r="D285" s="15"/>
     </row>
-    <row r="286" spans="1:4">
+    <row r="286" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A286" s="4" t="s">
         <v>1</v>
       </c>
@@ -5300,82 +4621,82 @@
         <v>4</v>
       </c>
     </row>
-    <row r="287" spans="1:4">
+    <row r="287" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A287" s="4"/>
       <c r="B287" t="s">
         <v>40</v>
       </c>
       <c r="D287" s="5" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="288" spans="1:4">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="288" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A288" s="4"/>
       <c r="B288" t="s">
         <v>43</v>
       </c>
       <c r="D288" s="5" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="289" spans="1:4">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="289" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A289" s="4"/>
       <c r="B289" t="s">
         <v>45</v>
       </c>
       <c r="D289" s="5" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="290" spans="1:4">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="290" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A290" s="4"/>
       <c r="B290" t="s">
         <v>47</v>
       </c>
       <c r="D290" s="5" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="291" spans="1:4">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="291" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A291" s="4"/>
       <c r="B291" t="s">
         <v>49</v>
       </c>
       <c r="D291" s="5" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="292" spans="1:4">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="292" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A292" s="4" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="B292" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="C292" t="s">
         <v>52</v>
       </c>
       <c r="D292" s="5" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="293" spans="1:4">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="293" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A293" s="4" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="B293" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C293" t="s">
         <v>52</v>
       </c>
       <c r="D293" s="24" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="294" spans="1:4">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="294" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A294" s="4" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="B294" t="s">
         <v>55</v>
@@ -5384,24 +4705,24 @@
         <v>52</v>
       </c>
       <c r="D294" s="5" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="295" spans="1:4">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="295" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A295" s="4" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="B295" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="C295" t="s">
         <v>7</v>
       </c>
       <c r="D295" s="5" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="296" ht="19.5" spans="1:4">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="296" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A296" s="17"/>
       <c r="B296" s="18" t="s">
         <v>20</v>
@@ -5409,17 +4730,15 @@
       <c r="C296" s="18"/>
       <c r="D296" s="19"/>
     </row>
-    <row r="297" ht="19.5"/>
-    <row r="298" ht="19.5"/>
-    <row r="299" ht="19.5" spans="1:4">
+    <row r="299" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A299" s="13" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B299" s="14"/>
       <c r="C299" s="14"/>
       <c r="D299" s="15"/>
     </row>
-    <row r="300" spans="1:4">
+    <row r="300" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A300" s="4" t="s">
         <v>1</v>
       </c>
@@ -5433,58 +4752,58 @@
         <v>4</v>
       </c>
     </row>
-    <row r="301" spans="1:4">
+    <row r="301" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A301" s="4" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B301" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="C301" t="s">
         <v>7</v>
       </c>
       <c r="D301" s="5" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="302" spans="1:4">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="302" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A302" s="4"/>
       <c r="B302" t="s">
         <v>10</v>
       </c>
       <c r="D302" s="5" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="303" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A303" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B303" t="s">
+        <v>294</v>
+      </c>
+      <c r="C303" t="s">
+        <v>171</v>
+      </c>
+      <c r="D303" s="5" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="304" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A304" s="4" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="303" spans="1:4">
-      <c r="A303" s="4" t="s">
+      <c r="B304" t="s">
         <v>297</v>
-      </c>
-      <c r="B303" t="s">
-        <v>298</v>
-      </c>
-      <c r="C303" t="s">
-        <v>175</v>
-      </c>
-      <c r="D303" s="5" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="304" spans="1:4">
-      <c r="A304" s="4" t="s">
-        <v>300</v>
-      </c>
-      <c r="B304" t="s">
-        <v>301</v>
       </c>
       <c r="C304" t="s">
         <v>18</v>
       </c>
       <c r="D304" s="5" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="305" spans="1:4">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="305" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A305" s="4"/>
       <c r="B305" t="s">
         <v>23</v>
@@ -5493,10 +4812,10 @@
         <v>24</v>
       </c>
       <c r="D305" s="5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="306" spans="1:4">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="306" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A306" s="4"/>
       <c r="B306" t="s">
         <v>27</v>
@@ -5506,7 +4825,7 @@
       </c>
       <c r="D306" s="5"/>
     </row>
-    <row r="307" ht="19.5" spans="1:4">
+    <row r="307" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A307" s="17"/>
       <c r="B307" s="18" t="s">
         <v>29</v>
@@ -5516,17 +4835,15 @@
       </c>
       <c r="D307" s="19"/>
     </row>
-    <row r="308" ht="19.5"/>
-    <row r="309" ht="19.5"/>
-    <row r="310" ht="19.5" spans="1:4">
+    <row r="310" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A310" s="13" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B310" s="14"/>
       <c r="C310" s="14"/>
       <c r="D310" s="15"/>
     </row>
-    <row r="311" spans="1:4">
+    <row r="311" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A311" s="4" t="s">
         <v>1</v>
       </c>
@@ -5540,122 +4857,122 @@
         <v>4</v>
       </c>
     </row>
-    <row r="312" spans="1:4">
+    <row r="312" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A312" s="4"/>
       <c r="B312" t="s">
         <v>40</v>
       </c>
       <c r="D312" s="5" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="313" spans="1:4">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="313" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A313" s="4"/>
       <c r="B313" t="s">
         <v>43</v>
       </c>
       <c r="D313" s="5" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="314" spans="1:4">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="314" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A314" s="4"/>
       <c r="B314" t="s">
         <v>45</v>
       </c>
       <c r="D314" s="5" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="315" spans="1:4">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="315" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A315" s="4"/>
       <c r="B315" t="s">
         <v>47</v>
       </c>
       <c r="D315" s="5" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="316" spans="1:4">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="316" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A316" s="4"/>
       <c r="B316" t="s">
         <v>49</v>
       </c>
       <c r="D316" s="5" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="317" spans="1:4">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="317" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A317" s="4" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B317" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C317" t="s">
         <v>52</v>
       </c>
       <c r="D317" s="5" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="318" spans="1:4">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="318" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A318" s="4" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="B318" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="C318" t="s">
         <v>52</v>
       </c>
       <c r="D318" s="5" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="319" spans="1:4">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="319" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A319" s="4" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="B319" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="C319" t="s">
         <v>52</v>
       </c>
       <c r="D319" s="20" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="320" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A320" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="B320" t="s">
+        <v>310</v>
+      </c>
+      <c r="C320" t="s">
+        <v>97</v>
+      </c>
+      <c r="D320" s="5" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="321" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A321" s="4" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="320" spans="1:4">
-      <c r="A320" s="4" t="s">
+      <c r="B321" t="s">
         <v>313</v>
       </c>
-      <c r="B320" t="s">
+      <c r="C321" t="s">
+        <v>97</v>
+      </c>
+      <c r="D321" s="20" t="s">
         <v>314</v>
       </c>
-      <c r="C320" t="s">
-        <v>101</v>
-      </c>
-      <c r="D320" s="5" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="321" spans="1:4">
-      <c r="A321" s="4" t="s">
-        <v>316</v>
-      </c>
-      <c r="B321" t="s">
-        <v>317</v>
-      </c>
-      <c r="C321" t="s">
-        <v>101</v>
-      </c>
-      <c r="D321" s="20" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="322" ht="19.5" spans="1:4">
+    </row>
+    <row r="322" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A322" s="17"/>
       <c r="B322" s="18" t="s">
         <v>20</v>
@@ -5663,17 +4980,15 @@
       <c r="C322" s="18"/>
       <c r="D322" s="19"/>
     </row>
-    <row r="323" ht="19.5"/>
-    <row r="324" ht="19.5"/>
-    <row r="325" ht="19.5" spans="1:4">
+    <row r="325" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A325" s="13" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B325" s="14"/>
       <c r="C325" s="14"/>
       <c r="D325" s="15"/>
     </row>
-    <row r="326" spans="1:4">
+    <row r="326" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A326" s="4" t="s">
         <v>1</v>
       </c>
@@ -5687,52 +5002,52 @@
         <v>4</v>
       </c>
     </row>
-    <row r="327" spans="1:4">
+    <row r="327" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A327" s="4" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B327" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C327" t="s">
         <v>7</v>
       </c>
       <c r="D327" s="5" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="328" spans="1:4">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="328" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A328" s="4"/>
       <c r="B328" t="s">
         <v>10</v>
       </c>
       <c r="D328" s="5" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="329" spans="1:4">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="329" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A329" s="4" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="B329" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D329" s="5" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="330" spans="1:4">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="330" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A330" s="4" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="B330" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="D330" s="5" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="331" spans="1:4">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="331" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A331" s="4"/>
       <c r="B331" t="s">
         <v>23</v>
@@ -5741,17 +5056,17 @@
         <v>24</v>
       </c>
       <c r="D331" s="5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="332" spans="1:4">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="332" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A332" s="4"/>
       <c r="B332" t="s">
         <v>27</v>
       </c>
       <c r="D332" s="5"/>
     </row>
-    <row r="333" ht="19.5" spans="1:4">
+    <row r="333" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A333" s="17"/>
       <c r="B333" s="18" t="s">
         <v>29</v>
@@ -5759,17 +5074,15 @@
       <c r="C333" s="18"/>
       <c r="D333" s="19"/>
     </row>
-    <row r="334" ht="19.5"/>
-    <row r="335" ht="19.5"/>
-    <row r="336" ht="19.5" spans="1:4">
+    <row r="336" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A336" s="13" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="B336" s="14"/>
       <c r="C336" s="14"/>
       <c r="D336" s="15"/>
     </row>
-    <row r="337" spans="1:4">
+    <row r="337" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A337" s="4" t="s">
         <v>1</v>
       </c>
@@ -5783,108 +5096,108 @@
         <v>4</v>
       </c>
     </row>
-    <row r="338" spans="1:4">
+    <row r="338" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A338" s="4"/>
       <c r="B338" t="s">
         <v>40</v>
       </c>
       <c r="D338" s="5" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="339" spans="1:4">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="339" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A339" s="4"/>
       <c r="B339" t="s">
         <v>43</v>
       </c>
       <c r="D339" s="5" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="340" spans="1:4">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="340" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A340" s="4"/>
       <c r="B340" t="s">
         <v>45</v>
       </c>
       <c r="D340" s="5" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="341" spans="1:4">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="341" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A341" s="4"/>
       <c r="B341" t="s">
         <v>47</v>
       </c>
       <c r="D341" s="5" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="342" spans="1:4">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="342" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A342" s="4"/>
       <c r="B342" t="s">
         <v>49</v>
       </c>
       <c r="D342" s="5" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="343" spans="1:4">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="343" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A343" s="4" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="B343" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="C343" t="s">
         <v>52</v>
       </c>
       <c r="D343" s="5" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="344" spans="1:4">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="344" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A344" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="B344" t="s">
+        <v>325</v>
+      </c>
+      <c r="C344" t="s">
+        <v>97</v>
+      </c>
+      <c r="D344" s="5" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="345" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A345" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="B345" t="s">
+        <v>327</v>
+      </c>
+      <c r="C345" t="s">
+        <v>97</v>
+      </c>
+      <c r="D345" s="20" t="s">
         <v>328</v>
       </c>
-      <c r="B344" t="s">
+    </row>
+    <row r="346" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A346" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="B346" t="s">
         <v>329</v>
-      </c>
-      <c r="C344" t="s">
-        <v>101</v>
-      </c>
-      <c r="D344" s="5" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="345" spans="1:4">
-      <c r="A345" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="B345" t="s">
-        <v>331</v>
-      </c>
-      <c r="C345" t="s">
-        <v>101</v>
-      </c>
-      <c r="D345" s="20" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="346" spans="1:4">
-      <c r="A346" s="4" t="s">
-        <v>324</v>
-      </c>
-      <c r="B346" t="s">
-        <v>333</v>
       </c>
       <c r="C346" t="s">
         <v>18</v>
       </c>
       <c r="D346" s="5" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="347" ht="19.5" spans="1:4">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="347" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A347" s="17"/>
       <c r="B347" s="18" t="s">
         <v>20</v>
@@ -5892,15 +5205,15 @@
       <c r="C347" s="18"/>
       <c r="D347" s="19"/>
     </row>
-    <row r="348" ht="19.5"/>
-    <row r="351" spans="1:4">
+    <row r="351" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A351" s="4"/>
       <c r="B351" s="16"/>
       <c r="C351" s="16"/>
       <c r="D351" s="5"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Change cangku page Ref #18
</commit_message>
<xml_diff>
--- a/database/数据库-业务处理.xlsx
+++ b/database/数据库-业务处理.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12195"/>
+    <workbookView windowWidth="11520" windowHeight="9300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="334">
   <si>
     <t>purchase_request表（请购单）</t>
   </si>
@@ -214,16 +214,13 @@
     <t>存货属性</t>
   </si>
   <si>
-    <t>ts_present_num</t>
+    <t>total_present_num</t>
   </si>
   <si>
     <t>center_stock表（中心存储物）</t>
   </si>
   <si>
     <t>仓库编号</t>
-  </si>
-  <si>
-    <t>cs_present_num</t>
   </si>
   <si>
     <t>purchase_contract表（采购合同）</t>
@@ -1554,8 +1551,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1563,6 +1569,21 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1576,14 +1597,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
@@ -1592,30 +1605,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1636,16 +1626,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1658,23 +1641,37 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -1692,7 +1689,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1707,7 +1704,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1719,19 +1764,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1743,7 +1818,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1761,37 +1872,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1803,91 +1884,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1981,20 +1978,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2004,6 +1998,47 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2025,56 +2060,18 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2083,148 +2080,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2307,54 +2304,54 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="1" builtinId="52"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="2" builtinId="42"/>
-    <cellStyle name="强调文字颜色 4" xfId="3" builtinId="41"/>
-    <cellStyle name="输入" xfId="4" builtinId="20"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="5" builtinId="39"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="6" builtinId="38"/>
-    <cellStyle name="货币" xfId="7" builtinId="4"/>
-    <cellStyle name="强调文字颜色 3" xfId="8" builtinId="37"/>
-    <cellStyle name="百分比" xfId="9" builtinId="5"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="10" builtinId="36"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="11" builtinId="48"/>
-    <cellStyle name="强调文字颜色 2" xfId="12" builtinId="33"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="13" builtinId="32"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="14" builtinId="44"/>
-    <cellStyle name="计算" xfId="15" builtinId="22"/>
-    <cellStyle name="强调文字颜色 1" xfId="16" builtinId="29"/>
-    <cellStyle name="适中" xfId="17" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="18" builtinId="46"/>
-    <cellStyle name="好" xfId="19" builtinId="26"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="20" builtinId="30"/>
-    <cellStyle name="汇总" xfId="21" builtinId="25"/>
-    <cellStyle name="差" xfId="22" builtinId="27"/>
-    <cellStyle name="检查单元格" xfId="23" builtinId="23"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
     <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="标题 1" xfId="25" builtinId="16"/>
-    <cellStyle name="解释性文本" xfId="26" builtinId="53"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="27" builtinId="34"/>
-    <cellStyle name="标题 4" xfId="28" builtinId="19"/>
-    <cellStyle name="货币[0]" xfId="29" builtinId="7"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="30" builtinId="43"/>
-    <cellStyle name="千位分隔" xfId="31" builtinId="3"/>
-    <cellStyle name="已访问的超链接" xfId="32" builtinId="9"/>
-    <cellStyle name="标题" xfId="33" builtinId="15"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="34" builtinId="35"/>
-    <cellStyle name="警告文本" xfId="35" builtinId="11"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
-    <cellStyle name="注释" xfId="37" builtinId="10"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="38" builtinId="50"/>
-    <cellStyle name="强调文字颜色 5" xfId="39" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="40" builtinId="51"/>
-    <cellStyle name="超链接" xfId="41" builtinId="8"/>
-    <cellStyle name="千位分隔[0]" xfId="42" builtinId="6"/>
-    <cellStyle name="标题 2" xfId="43" builtinId="17"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
     <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="标题 3" xfId="45" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
     <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="47" builtinId="31"/>
-    <cellStyle name="链接单元格" xfId="48" builtinId="24"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2625,20 +2622,20 @@
   <sheetPr/>
   <dimension ref="A1:F351"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A335" workbookViewId="0">
-      <selection activeCell="D352" sqref="A350:D352"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="31.125" customWidth="1"/>
+    <col min="1" max="1" width="31.1296296296296" customWidth="1"/>
     <col min="2" max="2" width="18.75" customWidth="1"/>
     <col min="3" max="3" width="16.5" customWidth="1"/>
-    <col min="4" max="4" width="43.625" customWidth="1"/>
-    <col min="6" max="6" width="29.875" customWidth="1"/>
+    <col min="4" max="4" width="43.6296296296296" customWidth="1"/>
+    <col min="6" max="6" width="29.8796296296296" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="19.5" spans="1:4">
+    <row r="1" ht="15.15" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2802,7 +2799,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" ht="19.5" spans="1:4">
+    <row r="14" ht="15.15" spans="1:4">
       <c r="A14" s="10" t="s">
         <v>36</v>
       </c>
@@ -2816,9 +2813,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" ht="19.5"/>
-    <row r="16" ht="19.5"/>
-    <row r="17" ht="19.5" spans="1:4">
+    <row r="15" ht="15.15"/>
+    <row r="16" ht="15.15"/>
+    <row r="17" ht="15.15" spans="1:4">
       <c r="A17" s="13" t="s">
         <v>38</v>
       </c>
@@ -2933,7 +2930,7 @@
       <c r="C26" s="16"/>
       <c r="D26" s="5"/>
     </row>
-    <row r="27" ht="19.5" spans="1:4">
+    <row r="27" ht="15.15" spans="1:4">
       <c r="A27" s="17" t="s">
         <v>58</v>
       </c>
@@ -2947,9 +2944,9 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" ht="19.5"/>
-    <row r="29" ht="19.5"/>
-    <row r="30" ht="19.5" spans="1:4">
+    <row r="28" ht="15.15"/>
+    <row r="29" ht="15.15"/>
+    <row r="30" ht="15.15" spans="1:4">
       <c r="A30" s="13" t="s">
         <v>62</v>
       </c>
@@ -3020,7 +3017,7 @@
       </c>
       <c r="D38" s="5"/>
     </row>
-    <row r="39" ht="19.5" spans="1:4">
+    <row r="39" spans="1:4">
       <c r="A39" s="17" t="s">
         <v>66</v>
       </c>
@@ -3032,11 +3029,11 @@
       </c>
       <c r="D39" s="19"/>
     </row>
-    <row r="40" ht="19.5" spans="2:2">
+    <row r="40" ht="15.15" spans="2:2">
       <c r="B40" s="16"/>
     </row>
-    <row r="41" ht="19.5"/>
-    <row r="42" ht="19.5" spans="1:4">
+    <row r="41" ht="15.15"/>
+    <row r="42" ht="15.15" spans="1:4">
       <c r="A42" s="13" t="s">
         <v>67</v>
       </c>
@@ -3107,10 +3104,8 @@
       </c>
       <c r="D50" s="5"/>
     </row>
-    <row r="51" ht="19.5" spans="1:4">
-      <c r="A51" s="17" t="s">
-        <v>69</v>
-      </c>
+    <row r="51" spans="1:4">
+      <c r="A51" s="17"/>
       <c r="B51" s="18" t="s">
         <v>55</v>
       </c>
@@ -3119,11 +3114,11 @@
       </c>
       <c r="D51" s="19"/>
     </row>
-    <row r="52" ht="19.5"/>
-    <row r="53" ht="19.5"/>
-    <row r="54" ht="19.5" spans="1:4">
+    <row r="52" ht="15.15"/>
+    <row r="53" ht="15.15"/>
+    <row r="54" ht="15.15" spans="1:4">
       <c r="A54" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B54" s="14"/>
       <c r="C54" s="14"/>
@@ -3145,16 +3140,16 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B56" t="s">
         <v>71</v>
-      </c>
-      <c r="B56" t="s">
-        <v>72</v>
       </c>
       <c r="C56" t="s">
         <v>7</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -3163,63 +3158,63 @@
         <v>10</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B58" t="s">
         <v>75</v>
-      </c>
-      <c r="B58" t="s">
-        <v>76</v>
       </c>
       <c r="C58" t="s">
         <v>11</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="4"/>
       <c r="B59" t="s">
+        <v>77</v>
+      </c>
+      <c r="D59" s="5" t="s">
         <v>78</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B60" t="s">
         <v>80</v>
-      </c>
-      <c r="B60" t="s">
-        <v>81</v>
       </c>
       <c r="C60" t="s">
         <v>18</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B61" t="s">
         <v>83</v>
       </c>
-      <c r="B61" t="s">
+      <c r="C61" t="s">
         <v>84</v>
       </c>
-      <c r="C61" t="s">
+      <c r="D61" s="20" t="s">
         <v>85</v>
-      </c>
-      <c r="D61" s="20" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B62" t="s">
         <v>20</v>
@@ -3231,7 +3226,7 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B63" t="s">
         <v>23</v>
@@ -3243,7 +3238,7 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B64" t="s">
         <v>27</v>
@@ -3253,23 +3248,23 @@
       </c>
       <c r="D64" s="5"/>
     </row>
-    <row r="65" ht="19.5" spans="1:4">
+    <row r="65" ht="15.15" spans="1:4">
       <c r="A65" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="B65" s="18" t="s">
         <v>90</v>
-      </c>
-      <c r="B65" s="18" t="s">
-        <v>91</v>
       </c>
       <c r="C65" s="18" t="s">
         <v>18</v>
       </c>
       <c r="D65" s="19"/>
     </row>
-    <row r="66" ht="19.5"/>
-    <row r="67" ht="19.5"/>
-    <row r="68" ht="19.5" spans="1:4">
+    <row r="66" ht="15.15"/>
+    <row r="67" ht="15.15"/>
+    <row r="68" ht="15.15" spans="1:4">
       <c r="A68" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B68" s="14"/>
       <c r="C68" s="14"/>
@@ -3327,94 +3322,94 @@
     <row r="75" spans="1:4">
       <c r="A75" s="4"/>
       <c r="B75" t="s">
+        <v>92</v>
+      </c>
+      <c r="D75" s="20" t="s">
         <v>93</v>
-      </c>
-      <c r="D75" s="20" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B76" t="s">
         <v>95</v>
       </c>
-      <c r="B76" t="s">
+      <c r="C76" t="s">
         <v>96</v>
       </c>
-      <c r="C76" t="s">
+      <c r="D76" s="20" t="s">
         <v>97</v>
-      </c>
-      <c r="D76" s="20" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B77" t="s">
         <v>99</v>
       </c>
-      <c r="B77" t="s">
+      <c r="C77" t="s">
         <v>100</v>
       </c>
-      <c r="C77" t="s">
+      <c r="D77" s="20" t="s">
         <v>101</v>
-      </c>
-      <c r="D77" s="20" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B78" t="s">
         <v>103</v>
       </c>
-      <c r="B78" t="s">
+      <c r="C78" t="s">
+        <v>100</v>
+      </c>
+      <c r="D78" s="20" t="s">
         <v>104</v>
-      </c>
-      <c r="C78" t="s">
-        <v>101</v>
-      </c>
-      <c r="D78" s="20" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B79" t="s">
         <v>106</v>
       </c>
-      <c r="B79" t="s">
+      <c r="C79" t="s">
+        <v>100</v>
+      </c>
+      <c r="D79" s="20" t="s">
         <v>107</v>
-      </c>
-      <c r="C79" t="s">
-        <v>101</v>
-      </c>
-      <c r="D79" s="20" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B80" t="s">
         <v>109</v>
       </c>
-      <c r="B80" t="s">
+      <c r="C80" t="s">
+        <v>100</v>
+      </c>
+      <c r="D80" s="20" t="s">
         <v>110</v>
-      </c>
-      <c r="C80" t="s">
-        <v>101</v>
-      </c>
-      <c r="D80" s="20" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B81" t="s">
         <v>112</v>
       </c>
-      <c r="B81" t="s">
+      <c r="C81" t="s">
+        <v>100</v>
+      </c>
+      <c r="D81" s="20" t="s">
         <v>113</v>
-      </c>
-      <c r="C81" t="s">
-        <v>101</v>
-      </c>
-      <c r="D81" s="20" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -3424,9 +3419,9 @@
       </c>
       <c r="D82" s="5"/>
     </row>
-    <row r="83" ht="19.5" spans="1:4">
+    <row r="83" ht="15.15" spans="1:4">
       <c r="A83" s="17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B83" s="18" t="s">
         <v>20</v>
@@ -3435,14 +3430,14 @@
         <v>21</v>
       </c>
       <c r="D83" s="19" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="84" ht="15.15"/>
+    <row r="85" ht="15.15"/>
+    <row r="86" ht="15.15" spans="1:4">
+      <c r="A86" s="13" t="s">
         <v>116</v>
-      </c>
-    </row>
-    <row r="84" ht="19.5"/>
-    <row r="85" ht="19.5"/>
-    <row r="86" ht="19.5" spans="1:4">
-      <c r="A86" s="13" t="s">
-        <v>117</v>
       </c>
       <c r="B86" s="14"/>
       <c r="C86" s="14"/>
@@ -3464,77 +3459,77 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B88" t="s">
         <v>118</v>
       </c>
-      <c r="B88" t="s">
+      <c r="C88" t="s">
+        <v>96</v>
+      </c>
+      <c r="D88" s="5" t="s">
         <v>119</v>
-      </c>
-      <c r="C88" t="s">
-        <v>97</v>
-      </c>
-      <c r="D88" s="5" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B89" t="s">
         <v>121</v>
       </c>
-      <c r="B89" t="s">
+      <c r="C89" t="s">
+        <v>96</v>
+      </c>
+      <c r="D89" s="20" t="s">
         <v>122</v>
-      </c>
-      <c r="C89" t="s">
-        <v>97</v>
-      </c>
-      <c r="D89" s="20" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B90" t="s">
         <v>124</v>
       </c>
-      <c r="B90" t="s">
+      <c r="C90" t="s">
+        <v>100</v>
+      </c>
+      <c r="D90" s="5" t="s">
         <v>125</v>
-      </c>
-      <c r="C90" t="s">
-        <v>101</v>
-      </c>
-      <c r="D90" s="5" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B91" t="s">
         <v>127</v>
       </c>
-      <c r="B91" t="s">
+      <c r="C91" t="s">
         <v>128</v>
       </c>
-      <c r="C91" t="s">
+      <c r="D91" s="5" t="s">
         <v>129</v>
-      </c>
-      <c r="D91" s="5" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B92" t="s">
         <v>131</v>
-      </c>
-      <c r="B92" t="s">
-        <v>132</v>
       </c>
       <c r="C92" t="s">
         <v>60</v>
       </c>
       <c r="D92" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="93" ht="15.15" spans="1:4">
+      <c r="A93" s="17" t="s">
         <v>133</v>
-      </c>
-    </row>
-    <row r="93" ht="19.5" spans="1:4">
-      <c r="A93" s="17" t="s">
-        <v>134</v>
       </c>
       <c r="B93" s="18" t="s">
         <v>20</v>
@@ -3543,14 +3538,14 @@
         <v>21</v>
       </c>
       <c r="D93" s="19" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="94" ht="15.15"/>
+    <row r="95" ht="15.15"/>
+    <row r="96" ht="15.15" spans="1:4">
+      <c r="A96" s="13" t="s">
         <v>135</v>
-      </c>
-    </row>
-    <row r="94" ht="19.5"/>
-    <row r="95" ht="19.5"/>
-    <row r="96" ht="19.5" spans="1:4">
-      <c r="A96" s="13" t="s">
-        <v>136</v>
       </c>
       <c r="B96" s="14"/>
       <c r="C96" s="14"/>
@@ -3572,16 +3567,16 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B98" t="s">
         <v>137</v>
-      </c>
-      <c r="B98" t="s">
-        <v>138</v>
       </c>
       <c r="C98" t="s">
         <v>7</v>
       </c>
       <c r="D98" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -3590,42 +3585,42 @@
         <v>10</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="4"/>
       <c r="B100" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D100" s="5"/>
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B101" t="s">
         <v>141</v>
-      </c>
-      <c r="B101" t="s">
-        <v>142</v>
       </c>
       <c r="C101" t="s">
         <v>18</v>
       </c>
       <c r="D101" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B102" t="s">
         <v>144</v>
       </c>
-      <c r="B102" t="s">
+      <c r="C102" t="s">
+        <v>100</v>
+      </c>
+      <c r="D102" s="20" t="s">
         <v>145</v>
-      </c>
-      <c r="C102" t="s">
-        <v>101</v>
-      </c>
-      <c r="D102" s="20" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -3637,21 +3632,21 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B104" t="s">
         <v>147</v>
-      </c>
-      <c r="B104" t="s">
-        <v>148</v>
       </c>
       <c r="C104" t="s">
         <v>7</v>
       </c>
       <c r="D104" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B105" t="s">
         <v>23</v>
@@ -3660,21 +3655,21 @@
         <v>24</v>
       </c>
       <c r="D105" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B106" t="s">
         <v>27</v>
       </c>
       <c r="D106" s="5"/>
     </row>
-    <row r="107" ht="19.5" spans="1:4">
+    <row r="107" ht="15.15" spans="1:4">
       <c r="A107" s="17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B107" s="18" t="s">
         <v>29</v>
@@ -3682,13 +3677,13 @@
       <c r="C107" s="18"/>
       <c r="D107" s="19"/>
     </row>
-    <row r="108" ht="19.5"/>
-    <row r="109" ht="19.5" spans="6:6">
+    <row r="108" ht="15.15"/>
+    <row r="109" ht="15.15" spans="6:6">
       <c r="F109" s="18"/>
     </row>
-    <row r="110" ht="19.5" spans="1:6">
+    <row r="110" ht="15.15" spans="1:6">
       <c r="A110" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B110" s="14"/>
       <c r="C110" s="14"/>
@@ -3760,118 +3755,118 @@
     <row r="117" spans="1:6">
       <c r="A117" s="4"/>
       <c r="B117" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D117" s="21" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E117" s="16"/>
       <c r="F117" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="118" spans="1:6">
       <c r="A118" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B118" t="s">
+        <v>95</v>
+      </c>
+      <c r="C118" t="s">
         <v>96</v>
       </c>
-      <c r="C118" t="s">
+      <c r="D118" s="21" t="s">
         <v>97</v>
-      </c>
-      <c r="D118" s="21" t="s">
-        <v>98</v>
       </c>
       <c r="E118" s="16"/>
       <c r="F118" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="119" spans="1:6">
       <c r="A119" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B119" t="s">
+        <v>99</v>
+      </c>
+      <c r="C119" t="s">
         <v>100</v>
       </c>
-      <c r="C119" t="s">
+      <c r="D119" s="21" t="s">
         <v>101</v>
-      </c>
-      <c r="D119" s="21" t="s">
-        <v>102</v>
       </c>
       <c r="E119" s="16"/>
       <c r="F119" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="120" spans="1:6">
       <c r="A120" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B120" t="s">
+        <v>103</v>
+      </c>
+      <c r="C120" t="s">
+        <v>100</v>
+      </c>
+      <c r="D120" s="21" t="s">
         <v>104</v>
-      </c>
-      <c r="C120" t="s">
-        <v>101</v>
-      </c>
-      <c r="D120" s="21" t="s">
-        <v>105</v>
       </c>
       <c r="E120" s="16"/>
       <c r="F120" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="121" spans="1:6">
       <c r="A121" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B121" t="s">
+        <v>106</v>
+      </c>
+      <c r="C121" t="s">
+        <v>100</v>
+      </c>
+      <c r="D121" s="21" t="s">
         <v>107</v>
-      </c>
-      <c r="C121" t="s">
-        <v>101</v>
-      </c>
-      <c r="D121" s="21" t="s">
-        <v>108</v>
       </c>
       <c r="E121" s="16"/>
       <c r="F121" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="122" spans="1:6">
       <c r="A122" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B122" t="s">
+        <v>109</v>
+      </c>
+      <c r="C122" t="s">
+        <v>100</v>
+      </c>
+      <c r="D122" s="21" t="s">
         <v>110</v>
-      </c>
-      <c r="C122" t="s">
-        <v>101</v>
-      </c>
-      <c r="D122" s="21" t="s">
-        <v>111</v>
       </c>
       <c r="E122" s="16"/>
       <c r="F122" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="123" spans="1:6">
       <c r="A123" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B123" t="s">
+        <v>112</v>
+      </c>
+      <c r="C123" t="s">
+        <v>100</v>
+      </c>
+      <c r="D123" s="21" t="s">
         <v>113</v>
-      </c>
-      <c r="C123" t="s">
-        <v>101</v>
-      </c>
-      <c r="D123" s="21" t="s">
-        <v>114</v>
       </c>
       <c r="E123" s="16"/>
       <c r="F123" s="5"/>
@@ -3882,14 +3877,14 @@
         <v>6</v>
       </c>
       <c r="D124" s="16" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E124" s="16"/>
       <c r="F124" s="5"/>
     </row>
-    <row r="125" ht="19.5" spans="1:6">
+    <row r="125" ht="15.15" spans="1:6">
       <c r="A125" s="17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B125" s="18" t="s">
         <v>20</v>
@@ -3898,16 +3893,16 @@
         <v>21</v>
       </c>
       <c r="D125" s="18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E125" s="18"/>
       <c r="F125" s="19"/>
     </row>
-    <row r="126" ht="19.5"/>
-    <row r="127" ht="19.5"/>
-    <row r="128" ht="19.5" spans="1:5">
+    <row r="126" ht="15.15"/>
+    <row r="127" ht="15.15"/>
+    <row r="128" ht="15.15" spans="1:5">
       <c r="A128" s="13" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B128" s="14"/>
       <c r="C128" s="14"/>
@@ -3931,16 +3926,16 @@
     </row>
     <row r="130" spans="1:5">
       <c r="A130" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="B130" t="s">
         <v>167</v>
-      </c>
-      <c r="B130" t="s">
-        <v>168</v>
       </c>
       <c r="C130" t="s">
         <v>7</v>
       </c>
       <c r="D130" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E130" s="5"/>
     </row>
@@ -3950,67 +3945,67 @@
         <v>10</v>
       </c>
       <c r="D131" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E131" s="5"/>
     </row>
     <row r="132" spans="1:5">
       <c r="A132" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="B132" t="s">
         <v>170</v>
-      </c>
-      <c r="B132" t="s">
-        <v>171</v>
       </c>
       <c r="C132" t="s">
         <v>24</v>
       </c>
       <c r="D132" s="22" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E132" s="5"/>
     </row>
     <row r="133" spans="1:5">
       <c r="A133" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="B133" t="s">
         <v>173</v>
       </c>
-      <c r="B133" t="s">
+      <c r="C133" t="s">
         <v>174</v>
       </c>
-      <c r="C133" t="s">
+      <c r="D133" t="s">
         <v>175</v>
-      </c>
-      <c r="D133" t="s">
-        <v>176</v>
       </c>
       <c r="E133" s="5"/>
     </row>
     <row r="134" spans="1:5">
       <c r="A134" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B134" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C134" t="s">
         <v>18</v>
       </c>
       <c r="D134" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E134" s="5"/>
     </row>
     <row r="135" spans="1:5">
       <c r="A135" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B135" t="s">
         <v>178</v>
       </c>
-      <c r="B135" t="s">
+      <c r="C135" t="s">
         <v>179</v>
       </c>
-      <c r="C135" t="s">
+      <c r="D135" t="s">
         <v>180</v>
-      </c>
-      <c r="D135" t="s">
-        <v>181</v>
       </c>
       <c r="E135" s="5"/>
     </row>
@@ -4030,7 +4025,7 @@
         <v>24</v>
       </c>
       <c r="D137" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E137" s="5"/>
     </row>
@@ -4041,7 +4036,7 @@
       </c>
       <c r="E138" s="5"/>
     </row>
-    <row r="139" ht="19.5" spans="1:5">
+    <row r="139" ht="15.15" spans="1:5">
       <c r="A139" s="17"/>
       <c r="B139" s="18" t="s">
         <v>29</v>
@@ -4050,11 +4045,11 @@
       <c r="D139" s="18"/>
       <c r="E139" s="19"/>
     </row>
-    <row r="140" ht="19.5"/>
-    <row r="141" ht="19.5"/>
-    <row r="142" ht="19.5" spans="1:4">
+    <row r="140" ht="15.15"/>
+    <row r="141" ht="15.15"/>
+    <row r="142" ht="15.15" spans="1:4">
       <c r="A142" s="13" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B142" s="14"/>
       <c r="C142" s="14"/>
@@ -4112,102 +4107,102 @@
     <row r="149" spans="1:4">
       <c r="A149" s="4"/>
       <c r="B149" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C149" t="s">
         <v>52</v>
       </c>
       <c r="D149" s="20" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B150" t="s">
+        <v>95</v>
+      </c>
+      <c r="C150" t="s">
         <v>96</v>
       </c>
-      <c r="C150" t="s">
+      <c r="D150" s="20" t="s">
         <v>97</v>
-      </c>
-      <c r="D150" s="20" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B151" t="s">
+        <v>99</v>
+      </c>
+      <c r="C151" t="s">
         <v>100</v>
       </c>
-      <c r="C151" t="s">
+      <c r="D151" s="20" t="s">
         <v>101</v>
-      </c>
-      <c r="D151" s="20" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="152" spans="1:4">
       <c r="A152" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B152" t="s">
+        <v>103</v>
+      </c>
+      <c r="C152" t="s">
+        <v>100</v>
+      </c>
+      <c r="D152" s="20" t="s">
         <v>104</v>
-      </c>
-      <c r="C152" t="s">
-        <v>101</v>
-      </c>
-      <c r="D152" s="20" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B153" t="s">
+        <v>106</v>
+      </c>
+      <c r="C153" t="s">
+        <v>100</v>
+      </c>
+      <c r="D153" s="20" t="s">
         <v>107</v>
-      </c>
-      <c r="C153" t="s">
-        <v>101</v>
-      </c>
-      <c r="D153" s="20" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="154" spans="1:4">
       <c r="A154" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B154" t="s">
+        <v>109</v>
+      </c>
+      <c r="C154" t="s">
+        <v>100</v>
+      </c>
+      <c r="D154" s="20" t="s">
         <v>110</v>
-      </c>
-      <c r="C154" t="s">
-        <v>101</v>
-      </c>
-      <c r="D154" s="20" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="155" spans="1:4">
       <c r="A155" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B155" t="s">
+        <v>112</v>
+      </c>
+      <c r="C155" t="s">
+        <v>100</v>
+      </c>
+      <c r="D155" s="20" t="s">
         <v>189</v>
       </c>
-      <c r="B155" t="s">
-        <v>113</v>
-      </c>
-      <c r="C155" t="s">
-        <v>101</v>
-      </c>
-      <c r="D155" s="20" t="s">
+    </row>
+    <row r="156" ht="15.15" spans="1:4">
+      <c r="A156" s="17" t="s">
         <v>190</v>
-      </c>
-    </row>
-    <row r="156" ht="19.5" spans="1:4">
-      <c r="A156" s="17" t="s">
-        <v>191</v>
       </c>
       <c r="B156" s="18" t="s">
         <v>20</v>
@@ -4216,14 +4211,14 @@
         <v>21</v>
       </c>
       <c r="D156" s="19" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="157" ht="15.15"/>
+    <row r="158" ht="15.15"/>
+    <row r="159" ht="15.15" spans="1:4">
+      <c r="A159" s="13" t="s">
         <v>192</v>
-      </c>
-    </row>
-    <row r="157" ht="19.5"/>
-    <row r="158" ht="19.5"/>
-    <row r="159" ht="19.5" spans="1:4">
-      <c r="A159" s="13" t="s">
-        <v>193</v>
       </c>
       <c r="B159" s="14"/>
       <c r="C159" s="14"/>
@@ -4245,16 +4240,16 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B161" t="s">
         <v>194</v>
-      </c>
-      <c r="B161" t="s">
-        <v>195</v>
       </c>
       <c r="C161" t="s">
         <v>7</v>
       </c>
       <c r="D161" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="162" spans="1:4">
@@ -4263,54 +4258,54 @@
         <v>10</v>
       </c>
       <c r="D162" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="B163" t="s">
         <v>197</v>
       </c>
-      <c r="B163" t="s">
-        <v>198</v>
-      </c>
       <c r="C163" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D163" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="164" spans="1:4">
       <c r="A164" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="B164" t="s">
         <v>199</v>
-      </c>
-      <c r="B164" t="s">
-        <v>200</v>
       </c>
       <c r="C164" t="s">
         <v>11</v>
       </c>
       <c r="D164" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="165" spans="1:4">
       <c r="A165" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="B165" t="s">
         <v>201</v>
-      </c>
-      <c r="B165" t="s">
-        <v>202</v>
       </c>
       <c r="C165" t="s">
         <v>18</v>
       </c>
       <c r="D165" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="166" spans="1:4">
       <c r="A166" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B166" t="s">
         <v>15</v>
@@ -4319,7 +4314,7 @@
         <v>11</v>
       </c>
       <c r="D166" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="167" spans="1:4">
@@ -4328,7 +4323,7 @@
         <v>20</v>
       </c>
       <c r="D167" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="168" spans="1:4">
@@ -4340,7 +4335,7 @@
         <v>24</v>
       </c>
       <c r="D168" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="169" spans="1:4">
@@ -4350,7 +4345,7 @@
       </c>
       <c r="D169" s="5"/>
     </row>
-    <row r="170" ht="19.5" spans="1:4">
+    <row r="170" ht="15.15" spans="1:4">
       <c r="A170" s="17"/>
       <c r="B170" s="18" t="s">
         <v>29</v>
@@ -4360,11 +4355,11 @@
       </c>
       <c r="D170" s="19"/>
     </row>
-    <row r="171" ht="19.5"/>
-    <row r="172" ht="19.5"/>
-    <row r="173" ht="19.5" spans="1:4">
+    <row r="171" ht="15.15"/>
+    <row r="172" ht="15.15"/>
+    <row r="173" ht="15.15" spans="1:4">
       <c r="A173" s="13" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B173" s="14"/>
       <c r="C173" s="14"/>
@@ -4386,7 +4381,7 @@
     </row>
     <row r="175" spans="1:4">
       <c r="A175" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B175" t="s">
         <v>40</v>
@@ -4433,21 +4428,21 @@
     </row>
     <row r="180" spans="1:4">
       <c r="A180" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="B180" t="s">
         <v>208</v>
-      </c>
-      <c r="B180" t="s">
-        <v>209</v>
       </c>
       <c r="C180" t="s">
         <v>52</v>
       </c>
       <c r="D180" s="20" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="181" spans="1:4">
       <c r="A181" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B181" t="s">
         <v>55</v>
@@ -4456,27 +4451,27 @@
         <v>52</v>
       </c>
       <c r="D181" s="5" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="182" ht="19.5" spans="1:4">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="182" ht="15.15" spans="1:4">
       <c r="A182" s="17"/>
       <c r="B182" s="18" t="s">
         <v>20</v>
       </c>
       <c r="C182" s="18"/>
       <c r="D182" s="19" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="183" ht="15.15"/>
+    <row r="184" ht="15.15"/>
+    <row r="185" ht="16.35" spans="1:4">
+      <c r="A185" s="13" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="183" ht="19.5"/>
-    <row r="184" ht="19.5"/>
-    <row r="185" ht="21.75" spans="1:4">
-      <c r="A185" s="13" t="s">
+      <c r="B185" s="23" t="s">
         <v>214</v>
-      </c>
-      <c r="B185" s="23" t="s">
-        <v>215</v>
       </c>
       <c r="C185" s="14"/>
       <c r="D185" s="15"/>
@@ -4497,16 +4492,16 @@
     </row>
     <row r="187" spans="1:4">
       <c r="A187" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B187" t="s">
         <v>216</v>
-      </c>
-      <c r="B187" t="s">
-        <v>217</v>
       </c>
       <c r="C187" t="s">
         <v>7</v>
       </c>
       <c r="D187" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="188" spans="1:4">
@@ -4515,49 +4510,49 @@
         <v>10</v>
       </c>
       <c r="D188" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="189" spans="1:4">
       <c r="A189" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B189" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C189" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D189" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="190" spans="1:4">
       <c r="A190" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B190" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C190" t="s">
         <v>11</v>
       </c>
       <c r="D190" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="191" spans="1:4">
       <c r="A191" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B191" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C191" t="s">
         <v>18</v>
       </c>
       <c r="D191" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="192" spans="1:4">
@@ -4566,26 +4561,26 @@
         <v>20</v>
       </c>
       <c r="D192" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="193" spans="1:4">
       <c r="A193" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="B193" t="s">
         <v>226</v>
-      </c>
-      <c r="B193" t="s">
-        <v>227</v>
       </c>
       <c r="C193" t="s">
         <v>7</v>
       </c>
       <c r="D193" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="194" spans="1:4">
       <c r="A194" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B194" t="s">
         <v>23</v>
@@ -4594,7 +4589,7 @@
         <v>24</v>
       </c>
       <c r="D194" s="24" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="195" spans="1:4">
@@ -4603,24 +4598,24 @@
         <v>27</v>
       </c>
       <c r="D195" s="24" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="196" ht="19.5" spans="1:4">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="196" ht="15.15" spans="1:4">
       <c r="A196" s="17"/>
       <c r="B196" s="18" t="s">
         <v>29</v>
       </c>
       <c r="C196" s="18"/>
       <c r="D196" s="19" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="197" ht="15.15"/>
+    <row r="198" ht="15.15"/>
+    <row r="199" ht="15.15" spans="1:4">
+      <c r="A199" s="13" t="s">
         <v>232</v>
-      </c>
-    </row>
-    <row r="197" ht="19.5"/>
-    <row r="198" ht="19.5"/>
-    <row r="199" ht="19.5" spans="1:4">
-      <c r="A199" s="13" t="s">
-        <v>233</v>
       </c>
       <c r="B199" s="14"/>
       <c r="C199" s="14"/>
@@ -4646,7 +4641,7 @@
         <v>40</v>
       </c>
       <c r="D201" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="202" spans="1:4">
@@ -4655,7 +4650,7 @@
         <v>43</v>
       </c>
       <c r="D202" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="203" spans="1:4">
@@ -4664,7 +4659,7 @@
         <v>45</v>
       </c>
       <c r="D203" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="204" spans="1:4">
@@ -4673,7 +4668,7 @@
         <v>47</v>
       </c>
       <c r="D204" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="205" spans="1:4">
@@ -4682,33 +4677,33 @@
         <v>49</v>
       </c>
       <c r="D205" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="206" spans="1:4">
       <c r="A206" s="4"/>
       <c r="B206" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D206" s="5" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="207" ht="19.5" spans="1:4">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="207" ht="15.15" spans="1:4">
       <c r="A207" s="17"/>
       <c r="B207" s="18" t="s">
         <v>20</v>
       </c>
       <c r="C207" s="18"/>
       <c r="D207" s="19" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="208" ht="15.15"/>
+    <row r="209" ht="15.15"/>
+    <row r="210" ht="15.15" spans="1:4">
+      <c r="A210" s="13" t="s">
         <v>234</v>
-      </c>
-    </row>
-    <row r="208" ht="19.5"/>
-    <row r="209" ht="19.5"/>
-    <row r="210" ht="19.5" spans="1:4">
-      <c r="A210" s="13" t="s">
-        <v>235</v>
       </c>
       <c r="B210" s="14"/>
       <c r="C210" s="14"/>
@@ -4730,16 +4725,16 @@
     </row>
     <row r="212" spans="1:4">
       <c r="A212" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B212" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C212" t="s">
         <v>7</v>
       </c>
       <c r="D212" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="213" spans="1:4">
@@ -4748,49 +4743,49 @@
         <v>10</v>
       </c>
       <c r="D213" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="214" spans="1:4">
       <c r="A214" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="B214" t="s">
+        <v>197</v>
+      </c>
+      <c r="C214" t="s">
+        <v>174</v>
+      </c>
+      <c r="D214" s="5" t="s">
         <v>239</v>
-      </c>
-      <c r="B214" t="s">
-        <v>198</v>
-      </c>
-      <c r="C214" t="s">
-        <v>175</v>
-      </c>
-      <c r="D214" s="5" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="215" spans="1:4">
       <c r="A215" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B215" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C215" t="s">
         <v>11</v>
       </c>
       <c r="D215" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="216" spans="1:4">
       <c r="A216" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B216" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C216" t="s">
         <v>18</v>
       </c>
       <c r="D216" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="217" spans="1:4">
@@ -4799,21 +4794,21 @@
         <v>20</v>
       </c>
       <c r="D217" s="24" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="218" spans="1:4">
       <c r="A218" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B218" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C218" t="s">
         <v>7</v>
       </c>
       <c r="D218" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="219" spans="1:4">
@@ -4825,7 +4820,7 @@
         <v>24</v>
       </c>
       <c r="D219" s="24" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="220" spans="1:4">
@@ -4835,7 +4830,7 @@
       </c>
       <c r="D220" s="5"/>
     </row>
-    <row r="221" ht="19.5" spans="1:4">
+    <row r="221" ht="15.15" spans="1:4">
       <c r="A221" s="17"/>
       <c r="B221" s="18" t="s">
         <v>29</v>
@@ -4843,11 +4838,11 @@
       <c r="C221" s="18"/>
       <c r="D221" s="19"/>
     </row>
-    <row r="222" ht="19.5"/>
-    <row r="223" ht="19.5"/>
-    <row r="224" ht="19.5" spans="1:4">
+    <row r="222" ht="15.15"/>
+    <row r="223" ht="15.15"/>
+    <row r="224" ht="15.15" spans="1:4">
       <c r="A224" s="13" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B224" s="14"/>
       <c r="C224" s="14"/>
@@ -4905,11 +4900,11 @@
     <row r="231" spans="1:4">
       <c r="A231" s="4"/>
       <c r="B231" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D231" s="5"/>
     </row>
-    <row r="232" ht="19.5" spans="1:4">
+    <row r="232" ht="15.15" spans="1:4">
       <c r="A232" s="17"/>
       <c r="B232" s="18" t="s">
         <v>20</v>
@@ -4917,11 +4912,11 @@
       <c r="C232" s="18"/>
       <c r="D232" s="19"/>
     </row>
-    <row r="233" ht="19.5"/>
-    <row r="247" ht="19.5"/>
-    <row r="248" ht="19.5" spans="1:4">
+    <row r="233" ht="15.15"/>
+    <row r="247" ht="15.15"/>
+    <row r="248" ht="15.15" spans="1:4">
       <c r="A248" s="13" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B248" s="14"/>
       <c r="C248" s="14"/>
@@ -4943,16 +4938,16 @@
     </row>
     <row r="250" spans="1:4">
       <c r="A250" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B250" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C250" t="s">
         <v>7</v>
       </c>
       <c r="D250" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="251" spans="1:4">
@@ -4961,54 +4956,54 @@
         <v>10</v>
       </c>
       <c r="D251" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="252" spans="1:4">
       <c r="A252" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="B252" t="s">
         <v>252</v>
       </c>
-      <c r="B252" t="s">
+      <c r="C252" t="s">
+        <v>174</v>
+      </c>
+      <c r="D252" s="5" t="s">
         <v>253</v>
-      </c>
-      <c r="C252" t="s">
-        <v>175</v>
-      </c>
-      <c r="D252" s="5" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="253" spans="1:4">
       <c r="A253" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="B253" t="s">
         <v>255</v>
       </c>
-      <c r="B253" t="s">
+      <c r="C253" t="s">
+        <v>174</v>
+      </c>
+      <c r="D253" s="20" t="s">
         <v>256</v>
-      </c>
-      <c r="C253" t="s">
-        <v>175</v>
-      </c>
-      <c r="D253" s="20" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="254" spans="1:4">
       <c r="A254" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="B254" t="s">
         <v>258</v>
-      </c>
-      <c r="B254" t="s">
-        <v>259</v>
       </c>
       <c r="C254" t="s">
         <v>18</v>
       </c>
       <c r="D254" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="255" spans="1:4">
       <c r="A255" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B255" t="s">
         <v>15</v>
@@ -5017,12 +5012,12 @@
         <v>11</v>
       </c>
       <c r="D255" s="5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="256" spans="1:4">
       <c r="A256" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B256" t="s">
         <v>23</v>
@@ -5031,7 +5026,7 @@
         <v>24</v>
       </c>
       <c r="D256" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="257" spans="1:4">
@@ -5041,7 +5036,7 @@
       </c>
       <c r="D257" s="5"/>
     </row>
-    <row r="258" ht="19.5" spans="1:4">
+    <row r="258" ht="15.15" spans="1:4">
       <c r="A258" s="17"/>
       <c r="B258" s="18" t="s">
         <v>29</v>
@@ -5049,11 +5044,11 @@
       <c r="C258" s="18"/>
       <c r="D258" s="19"/>
     </row>
-    <row r="259" ht="19.5"/>
-    <row r="260" ht="19.5"/>
-    <row r="261" ht="19.5" spans="1:4">
+    <row r="259" ht="15.15"/>
+    <row r="260" ht="15.15"/>
+    <row r="261" ht="15.15" spans="1:4">
       <c r="A261" s="13" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B261" s="14"/>
       <c r="C261" s="14"/>
@@ -5079,7 +5074,7 @@
         <v>40</v>
       </c>
       <c r="D263" s="24" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="264" spans="1:4">
@@ -5088,7 +5083,7 @@
         <v>43</v>
       </c>
       <c r="D264" s="24" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="265" spans="1:4">
@@ -5097,7 +5092,7 @@
         <v>45</v>
       </c>
       <c r="D265" s="24" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="266" spans="1:4">
@@ -5106,7 +5101,7 @@
         <v>47</v>
       </c>
       <c r="D266" s="24" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="267" spans="1:4">
@@ -5115,26 +5110,26 @@
         <v>49</v>
       </c>
       <c r="D267" s="24" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="268" spans="1:4">
       <c r="A268" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="B268" t="s">
         <v>265</v>
-      </c>
-      <c r="B268" t="s">
-        <v>266</v>
       </c>
       <c r="C268" t="s">
         <v>52</v>
       </c>
       <c r="D268" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="269" spans="1:4">
       <c r="A269" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B269" t="s">
         <v>55</v>
@@ -5143,10 +5138,10 @@
         <v>52</v>
       </c>
       <c r="D269" s="24" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="270" ht="19.5" spans="1:4">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="270" ht="15.15" spans="1:4">
       <c r="A270" s="17"/>
       <c r="B270" s="18" t="s">
         <v>20</v>
@@ -5154,11 +5149,11 @@
       <c r="C270" s="18"/>
       <c r="D270" s="19"/>
     </row>
-    <row r="271" ht="19.5"/>
-    <row r="272" ht="19.5"/>
-    <row r="273" ht="19.5" spans="1:4">
+    <row r="271" ht="15.15"/>
+    <row r="272" ht="15.15"/>
+    <row r="273" ht="15.15" spans="1:4">
       <c r="A273" s="13" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B273" s="14"/>
       <c r="C273" s="14"/>
@@ -5180,16 +5175,16 @@
     </row>
     <row r="275" spans="1:4">
       <c r="A275" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B275" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C275" t="s">
         <v>7</v>
       </c>
       <c r="D275" s="5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="276" ht="19" customHeight="1" spans="1:4">
@@ -5198,49 +5193,49 @@
         <v>10</v>
       </c>
       <c r="D276" s="5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="277" spans="1:4">
       <c r="A277" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="B277" t="s">
+        <v>252</v>
+      </c>
+      <c r="C277" t="s">
+        <v>174</v>
+      </c>
+      <c r="D277" s="5" t="s">
         <v>274</v>
-      </c>
-      <c r="B277" t="s">
-        <v>253</v>
-      </c>
-      <c r="C277" t="s">
-        <v>175</v>
-      </c>
-      <c r="D277" s="5" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="278" spans="1:4">
       <c r="A278" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B278" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C278" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D278" s="5" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="279" spans="1:4">
       <c r="A279" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B279" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C279" t="s">
         <v>18</v>
       </c>
       <c r="D279" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="280" spans="1:4">
@@ -5252,7 +5247,7 @@
         <v>24</v>
       </c>
       <c r="D280" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="281" spans="1:4">
@@ -5261,26 +5256,26 @@
         <v>27</v>
       </c>
       <c r="D281" s="5" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="282" ht="15.15" spans="1:4">
+      <c r="A282" s="17" t="s">
         <v>278</v>
-      </c>
-    </row>
-    <row r="282" ht="19.5" spans="1:4">
-      <c r="A282" s="17" t="s">
-        <v>279</v>
       </c>
       <c r="B282" s="18" t="s">
         <v>29</v>
       </c>
       <c r="C282" s="18"/>
       <c r="D282" s="19" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="283" ht="15.15"/>
+    <row r="284" ht="15.15"/>
+    <row r="285" ht="15.15" spans="1:4">
+      <c r="A285" s="13" t="s">
         <v>280</v>
-      </c>
-    </row>
-    <row r="283" ht="19.5"/>
-    <row r="284" ht="19.5"/>
-    <row r="285" ht="19.5" spans="1:4">
-      <c r="A285" s="13" t="s">
-        <v>281</v>
       </c>
       <c r="B285" s="14"/>
       <c r="C285" s="14"/>
@@ -5306,7 +5301,7 @@
         <v>40</v>
       </c>
       <c r="D287" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="288" spans="1:4">
@@ -5315,7 +5310,7 @@
         <v>43</v>
       </c>
       <c r="D288" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="289" spans="1:4">
@@ -5324,7 +5319,7 @@
         <v>45</v>
       </c>
       <c r="D289" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="290" spans="1:4">
@@ -5333,7 +5328,7 @@
         <v>47</v>
       </c>
       <c r="D290" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="291" spans="1:4">
@@ -5342,40 +5337,40 @@
         <v>49</v>
       </c>
       <c r="D291" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="292" spans="1:4">
       <c r="A292" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B292" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C292" t="s">
         <v>52</v>
       </c>
       <c r="D292" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="293" spans="1:4">
       <c r="A293" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="B293" t="s">
         <v>284</v>
-      </c>
-      <c r="B293" t="s">
-        <v>285</v>
       </c>
       <c r="C293" t="s">
         <v>52</v>
       </c>
       <c r="D293" s="24" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="294" spans="1:4">
       <c r="A294" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B294" t="s">
         <v>55</v>
@@ -5384,24 +5379,24 @@
         <v>52</v>
       </c>
       <c r="D294" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="295" spans="1:4">
       <c r="A295" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="B295" t="s">
         <v>289</v>
-      </c>
-      <c r="B295" t="s">
-        <v>290</v>
       </c>
       <c r="C295" t="s">
         <v>7</v>
       </c>
       <c r="D295" s="5" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="296" ht="19.5" spans="1:4">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="296" ht="15.15" spans="1:4">
       <c r="A296" s="17"/>
       <c r="B296" s="18" t="s">
         <v>20</v>
@@ -5409,11 +5404,11 @@
       <c r="C296" s="18"/>
       <c r="D296" s="19"/>
     </row>
-    <row r="297" ht="19.5"/>
-    <row r="298" ht="19.5"/>
-    <row r="299" ht="19.5" spans="1:4">
+    <row r="297" ht="15.15"/>
+    <row r="298" ht="15.15"/>
+    <row r="299" ht="15.15" spans="1:4">
       <c r="A299" s="13" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B299" s="14"/>
       <c r="C299" s="14"/>
@@ -5435,16 +5430,16 @@
     </row>
     <row r="301" spans="1:4">
       <c r="A301" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="B301" t="s">
         <v>293</v>
-      </c>
-      <c r="B301" t="s">
-        <v>294</v>
       </c>
       <c r="C301" t="s">
         <v>7</v>
       </c>
       <c r="D301" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="302" spans="1:4">
@@ -5453,35 +5448,35 @@
         <v>10</v>
       </c>
       <c r="D302" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="303" spans="1:4">
       <c r="A303" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="B303" t="s">
         <v>297</v>
       </c>
-      <c r="B303" t="s">
+      <c r="C303" t="s">
+        <v>174</v>
+      </c>
+      <c r="D303" s="5" t="s">
         <v>298</v>
-      </c>
-      <c r="C303" t="s">
-        <v>175</v>
-      </c>
-      <c r="D303" s="5" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="304" spans="1:4">
       <c r="A304" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="B304" t="s">
         <v>300</v>
-      </c>
-      <c r="B304" t="s">
-        <v>301</v>
       </c>
       <c r="C304" t="s">
         <v>18</v>
       </c>
       <c r="D304" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="305" spans="1:4">
@@ -5493,7 +5488,7 @@
         <v>24</v>
       </c>
       <c r="D305" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="306" spans="1:4">
@@ -5506,7 +5501,7 @@
       </c>
       <c r="D306" s="5"/>
     </row>
-    <row r="307" ht="19.5" spans="1:4">
+    <row r="307" ht="15.15" spans="1:4">
       <c r="A307" s="17"/>
       <c r="B307" s="18" t="s">
         <v>29</v>
@@ -5516,11 +5511,11 @@
       </c>
       <c r="D307" s="19"/>
     </row>
-    <row r="308" ht="19.5"/>
-    <row r="309" ht="19.5"/>
-    <row r="310" ht="19.5" spans="1:4">
+    <row r="308" ht="15.15"/>
+    <row r="309" ht="15.15"/>
+    <row r="310" ht="15.15" spans="1:4">
       <c r="A310" s="13" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B310" s="14"/>
       <c r="C310" s="14"/>
@@ -5546,7 +5541,7 @@
         <v>40</v>
       </c>
       <c r="D312" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="313" spans="1:4">
@@ -5555,7 +5550,7 @@
         <v>43</v>
       </c>
       <c r="D313" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="314" spans="1:4">
@@ -5564,7 +5559,7 @@
         <v>45</v>
       </c>
       <c r="D314" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="315" spans="1:4">
@@ -5573,7 +5568,7 @@
         <v>47</v>
       </c>
       <c r="D315" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="316" spans="1:4">
@@ -5582,80 +5577,80 @@
         <v>49</v>
       </c>
       <c r="D316" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="317" spans="1:4">
       <c r="A317" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B317" t="s">
         <v>304</v>
-      </c>
-      <c r="B317" t="s">
-        <v>305</v>
       </c>
       <c r="C317" t="s">
         <v>52</v>
       </c>
       <c r="D317" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="318" spans="1:4">
       <c r="A318" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="B318" t="s">
         <v>307</v>
-      </c>
-      <c r="B318" t="s">
-        <v>308</v>
       </c>
       <c r="C318" t="s">
         <v>52</v>
       </c>
       <c r="D318" s="5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="319" spans="1:4">
       <c r="A319" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="B319" t="s">
         <v>310</v>
-      </c>
-      <c r="B319" t="s">
-        <v>311</v>
       </c>
       <c r="C319" t="s">
         <v>52</v>
       </c>
       <c r="D319" s="20" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="320" spans="1:4">
       <c r="A320" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B320" t="s">
         <v>313</v>
       </c>
-      <c r="B320" t="s">
+      <c r="C320" t="s">
+        <v>100</v>
+      </c>
+      <c r="D320" s="5" t="s">
         <v>314</v>
-      </c>
-      <c r="C320" t="s">
-        <v>101</v>
-      </c>
-      <c r="D320" s="5" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="321" spans="1:4">
       <c r="A321" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="B321" t="s">
         <v>316</v>
       </c>
-      <c r="B321" t="s">
+      <c r="C321" t="s">
+        <v>100</v>
+      </c>
+      <c r="D321" s="20" t="s">
         <v>317</v>
       </c>
-      <c r="C321" t="s">
-        <v>101</v>
-      </c>
-      <c r="D321" s="20" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="322" ht="19.5" spans="1:4">
+    </row>
+    <row r="322" ht="15.15" spans="1:4">
       <c r="A322" s="17"/>
       <c r="B322" s="18" t="s">
         <v>20</v>
@@ -5663,11 +5658,11 @@
       <c r="C322" s="18"/>
       <c r="D322" s="19"/>
     </row>
-    <row r="323" ht="19.5"/>
-    <row r="324" ht="19.5"/>
-    <row r="325" ht="19.5" spans="1:4">
+    <row r="323" ht="15.15"/>
+    <row r="324" ht="15.15"/>
+    <row r="325" ht="15.15" spans="1:4">
       <c r="A325" s="13" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B325" s="14"/>
       <c r="C325" s="14"/>
@@ -5689,16 +5684,16 @@
     </row>
     <row r="327" spans="1:4">
       <c r="A327" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="B327" t="s">
         <v>320</v>
-      </c>
-      <c r="B327" t="s">
-        <v>321</v>
       </c>
       <c r="C327" t="s">
         <v>7</v>
       </c>
       <c r="D327" s="5" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="328" spans="1:4">
@@ -5707,29 +5702,29 @@
         <v>10</v>
       </c>
       <c r="D328" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="329" spans="1:4">
       <c r="A329" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B329" t="s">
+        <v>297</v>
+      </c>
+      <c r="D329" s="5" t="s">
         <v>298</v>
-      </c>
-      <c r="D329" s="5" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="330" spans="1:4">
       <c r="A330" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B330" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D330" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="331" spans="1:4">
@@ -5741,7 +5736,7 @@
         <v>24</v>
       </c>
       <c r="D331" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="332" spans="1:4">
@@ -5751,7 +5746,7 @@
       </c>
       <c r="D332" s="5"/>
     </row>
-    <row r="333" ht="19.5" spans="1:4">
+    <row r="333" ht="15.15" spans="1:4">
       <c r="A333" s="17"/>
       <c r="B333" s="18" t="s">
         <v>29</v>
@@ -5759,11 +5754,11 @@
       <c r="C333" s="18"/>
       <c r="D333" s="19"/>
     </row>
-    <row r="334" ht="19.5"/>
-    <row r="335" ht="19.5"/>
-    <row r="336" ht="19.5" spans="1:4">
+    <row r="334" ht="15.15"/>
+    <row r="335" ht="15.15"/>
+    <row r="336" ht="15.15" spans="1:4">
       <c r="A336" s="13" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B336" s="14"/>
       <c r="C336" s="14"/>
@@ -5789,7 +5784,7 @@
         <v>40</v>
       </c>
       <c r="D338" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="339" spans="1:4">
@@ -5798,7 +5793,7 @@
         <v>43</v>
       </c>
       <c r="D339" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="340" spans="1:4">
@@ -5807,7 +5802,7 @@
         <v>45</v>
       </c>
       <c r="D340" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="341" spans="1:4">
@@ -5816,7 +5811,7 @@
         <v>47</v>
       </c>
       <c r="D341" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="342" spans="1:4">
@@ -5825,66 +5820,66 @@
         <v>49</v>
       </c>
       <c r="D342" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="343" spans="1:4">
       <c r="A343" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="B343" t="s">
         <v>326</v>
-      </c>
-      <c r="B343" t="s">
-        <v>327</v>
       </c>
       <c r="C343" t="s">
         <v>52</v>
       </c>
       <c r="D343" s="5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="344" spans="1:4">
       <c r="A344" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="B344" t="s">
         <v>328</v>
       </c>
-      <c r="B344" t="s">
-        <v>329</v>
-      </c>
       <c r="C344" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D344" s="5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="345" spans="1:4">
       <c r="A345" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="B345" t="s">
         <v>330</v>
       </c>
-      <c r="B345" t="s">
+      <c r="C345" t="s">
+        <v>100</v>
+      </c>
+      <c r="D345" s="20" t="s">
         <v>331</v>
-      </c>
-      <c r="C345" t="s">
-        <v>101</v>
-      </c>
-      <c r="D345" s="20" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="346" spans="1:4">
       <c r="A346" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B346" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C346" t="s">
         <v>18</v>
       </c>
       <c r="D346" s="5" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="347" ht="19.5" spans="1:4">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="347" ht="15.15" spans="1:4">
       <c r="A347" s="17"/>
       <c r="B347" s="18" t="s">
         <v>20</v>
@@ -5892,7 +5887,7 @@
       <c r="C347" s="18"/>
       <c r="D347" s="19"/>
     </row>
-    <row r="348" ht="19.5"/>
+    <row r="348" ht="15.15"/>
     <row r="351" spans="1:4">
       <c r="A351" s="4"/>
       <c r="B351" s="16"/>

</xml_diff>